<commit_message>
:package: função fuzzy melhorada, mas ta considerando apenas a distribuição normal, portanto as vezes fica presa em outliers
</commit_message>
<xml_diff>
--- a/correlacao.xlsx
+++ b/correlacao.xlsx
@@ -524,7 +524,7 @@
         <v>0.230185825566185</v>
       </c>
       <c r="T2" t="n">
-        <v>0.0337162987150283</v>
+        <v>0.0337525921132433</v>
       </c>
     </row>
     <row r="3">
@@ -586,7 +586,7 @@
         <v>0.00375600238941258</v>
       </c>
       <c r="T3" t="n">
-        <v>-0.0524378460457139</v>
+        <v>-0.00102444424694228</v>
       </c>
     </row>
     <row r="4">
@@ -648,7 +648,7 @@
         <v>0.454460736719593</v>
       </c>
       <c r="T4" t="n">
-        <v>0.0950678618967026</v>
+        <v>0.0736324550142593</v>
       </c>
     </row>
     <row r="5">
@@ -710,7 +710,7 @@
         <v>0.0141993796528666</v>
       </c>
       <c r="T5" t="n">
-        <v>-0.0583632474556652</v>
+        <v>-0.0493644672164725</v>
       </c>
     </row>
     <row r="6">
@@ -772,7 +772,7 @@
         <v>0.00386004586622592</v>
       </c>
       <c r="T6" t="n">
-        <v>-0.0375974261238516</v>
+        <v>-0.0411602433657146</v>
       </c>
     </row>
     <row r="7">
@@ -834,7 +834,7 @@
         <v>0.0281147148177403</v>
       </c>
       <c r="T7" t="n">
-        <v>-0.0719312141648766</v>
+        <v>-0.121544158018929</v>
       </c>
     </row>
     <row r="8">
@@ -896,7 +896,7 @@
         <v>0.035893330194749</v>
       </c>
       <c r="T8" t="n">
-        <v>0.174723483589832</v>
+        <v>0.112519738309319</v>
       </c>
     </row>
     <row r="9">
@@ -958,7 +958,7 @@
         <v>0.0112143846899017</v>
       </c>
       <c r="T9" t="n">
-        <v>0.0900820445978703</v>
+        <v>0.0283522521926804</v>
       </c>
     </row>
     <row r="10">
@@ -1020,7 +1020,7 @@
         <v>-0.454845682066813</v>
       </c>
       <c r="T10" t="n">
-        <v>0.16841731700667</v>
+        <v>0.0552313760906616</v>
       </c>
     </row>
     <row r="11">
@@ -1082,7 +1082,7 @@
         <v>-0.134781477086767</v>
       </c>
       <c r="T11" t="n">
-        <v>-0.0450823004191116</v>
+        <v>-0.0360267154150473</v>
       </c>
     </row>
     <row r="12">
@@ -1144,7 +1144,7 @@
         <v>0.00277334363294089</v>
       </c>
       <c r="T12" t="n">
-        <v>0.0284887222315478</v>
+        <v>0.0182946147753705</v>
       </c>
     </row>
     <row r="13">
@@ -1206,7 +1206,7 @@
         <v>0.00384671931740002</v>
       </c>
       <c r="T13" t="n">
-        <v>0.0317962733305107</v>
+        <v>0.0206824311319558</v>
       </c>
     </row>
     <row r="14">
@@ -1268,7 +1268,7 @@
         <v>0.00455240045961079</v>
       </c>
       <c r="T14" t="n">
-        <v>-0.0212086788334043</v>
+        <v>-0.0179937388482054</v>
       </c>
     </row>
     <row r="15">
@@ -1330,7 +1330,7 @@
         <v>0.00233847014267316</v>
       </c>
       <c r="T15" t="n">
-        <v>0.0254562113168361</v>
+        <v>0.0276292582147641</v>
       </c>
     </row>
     <row r="16">
@@ -1392,7 +1392,7 @@
         <v>0.00109032845217988</v>
       </c>
       <c r="T16" t="n">
-        <v>-0.0213186066710558</v>
+        <v>0.0197943510483599</v>
       </c>
     </row>
     <row r="17">
@@ -1454,7 +1454,7 @@
         <v>0.0179464862953829</v>
       </c>
       <c r="T17" t="n">
-        <v>-0.0432162300934777</v>
+        <v>-0.0426506428566784</v>
       </c>
     </row>
     <row r="18">
@@ -1516,7 +1516,7 @@
         <v>0.228611505321296</v>
       </c>
       <c r="T18" t="n">
-        <v>0.0131041969669557</v>
+        <v>-0.000932168280232888</v>
       </c>
     </row>
     <row r="19">
@@ -1578,7 +1578,7 @@
         <v>0.00620459115425521</v>
       </c>
       <c r="T19" t="n">
-        <v>0.0056408383432696</v>
+        <v>-0.0143321336842633</v>
       </c>
     </row>
     <row r="20">
@@ -1640,66 +1640,66 @@
         <v>1</v>
       </c>
       <c r="T20" t="n">
-        <v>0.113240877584873</v>
+        <v>0.0635166560920207</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>0.0337162987150283</v>
+        <v>0.0337525921132433</v>
       </c>
       <c r="B21" t="n">
-        <v>-0.0524378460457139</v>
+        <v>-0.00102444424694228</v>
       </c>
       <c r="C21" t="n">
-        <v>0.0950678618967026</v>
+        <v>0.0736324550142593</v>
       </c>
       <c r="D21" t="n">
-        <v>-0.0583632474556652</v>
+        <v>-0.0493644672164725</v>
       </c>
       <c r="E21" t="n">
-        <v>-0.0375974261238516</v>
+        <v>-0.0411602433657146</v>
       </c>
       <c r="F21" t="n">
-        <v>-0.0719312141648766</v>
+        <v>-0.121544158018929</v>
       </c>
       <c r="G21" t="n">
-        <v>0.174723483589832</v>
+        <v>0.112519738309319</v>
       </c>
       <c r="H21" t="n">
-        <v>0.0900820445978703</v>
+        <v>0.0283522521926804</v>
       </c>
       <c r="I21" t="n">
-        <v>0.16841731700667</v>
+        <v>0.0552313760906616</v>
       </c>
       <c r="J21" t="n">
-        <v>-0.0450823004191116</v>
+        <v>-0.0360267154150473</v>
       </c>
       <c r="K21" t="n">
-        <v>0.0284887222315478</v>
+        <v>0.0182946147753705</v>
       </c>
       <c r="L21" t="n">
-        <v>0.0317962733305107</v>
+        <v>0.0206824311319558</v>
       </c>
       <c r="M21" t="n">
-        <v>-0.0212086788334043</v>
+        <v>-0.0179937388482054</v>
       </c>
       <c r="N21" t="n">
-        <v>0.0254562113168361</v>
+        <v>0.0276292582147641</v>
       </c>
       <c r="O21" t="n">
-        <v>-0.0213186066710558</v>
+        <v>0.0197943510483599</v>
       </c>
       <c r="P21" t="n">
-        <v>-0.0432162300934777</v>
+        <v>-0.0426506428566784</v>
       </c>
       <c r="Q21" t="n">
-        <v>0.0131041969669557</v>
+        <v>-0.000932168280232888</v>
       </c>
       <c r="R21" t="n">
-        <v>0.0056408383432696</v>
+        <v>-0.0143321336842633</v>
       </c>
       <c r="S21" t="n">
-        <v>0.113240877584873</v>
+        <v>0.0635166560920207</v>
       </c>
       <c r="T21" t="n">
         <v>1</v>

</xml_diff>

<commit_message>
:up: improve lookning for param, bef clean
</commit_message>
<xml_diff>
--- a/correlacao.xlsx
+++ b/correlacao.xlsx
@@ -524,7 +524,7 @@
         <v>0.230185825566185</v>
       </c>
       <c r="T2" t="n">
-        <v>0.0337525921132433</v>
+        <v>0.0287303267030508</v>
       </c>
     </row>
     <row r="3">
@@ -586,7 +586,7 @@
         <v>0.00375600238941258</v>
       </c>
       <c r="T3" t="n">
-        <v>-0.00102444424694228</v>
+        <v>-0.00495230430079656</v>
       </c>
     </row>
     <row r="4">
@@ -648,7 +648,7 @@
         <v>0.454460736719593</v>
       </c>
       <c r="T4" t="n">
-        <v>0.0736324550142593</v>
+        <v>0.0678001612532612</v>
       </c>
     </row>
     <row r="5">
@@ -710,7 +710,7 @@
         <v>0.0141993796528666</v>
       </c>
       <c r="T5" t="n">
-        <v>-0.0493644672164725</v>
+        <v>-0.0467775591202038</v>
       </c>
     </row>
     <row r="6">
@@ -772,7 +772,7 @@
         <v>0.00386004586622592</v>
       </c>
       <c r="T6" t="n">
-        <v>-0.0411602433657146</v>
+        <v>-0.0391769925902026</v>
       </c>
     </row>
     <row r="7">
@@ -834,7 +834,7 @@
         <v>0.0281147148177403</v>
       </c>
       <c r="T7" t="n">
-        <v>-0.121544158018929</v>
+        <v>-0.120653422087976</v>
       </c>
     </row>
     <row r="8">
@@ -896,7 +896,7 @@
         <v>0.035893330194749</v>
       </c>
       <c r="T8" t="n">
-        <v>0.112519738309319</v>
+        <v>0.11449442715349</v>
       </c>
     </row>
     <row r="9">
@@ -958,7 +958,7 @@
         <v>0.0112143846899017</v>
       </c>
       <c r="T9" t="n">
-        <v>0.0283522521926804</v>
+        <v>0.030974312496068</v>
       </c>
     </row>
     <row r="10">
@@ -1020,7 +1020,7 @@
         <v>-0.454845682066813</v>
       </c>
       <c r="T10" t="n">
-        <v>0.0552313760906616</v>
+        <v>0.0616668743602804</v>
       </c>
     </row>
     <row r="11">
@@ -1082,7 +1082,7 @@
         <v>-0.134781477086767</v>
       </c>
       <c r="T11" t="n">
-        <v>-0.0360267154150473</v>
+        <v>-0.0260576414308473</v>
       </c>
     </row>
     <row r="12">
@@ -1144,7 +1144,7 @@
         <v>0.00277334363294089</v>
       </c>
       <c r="T12" t="n">
-        <v>0.0182946147753705</v>
+        <v>0.0185889501276473</v>
       </c>
     </row>
     <row r="13">
@@ -1206,7 +1206,7 @@
         <v>0.00384671931740002</v>
       </c>
       <c r="T13" t="n">
-        <v>0.0206824311319558</v>
+        <v>0.0205364503277865</v>
       </c>
     </row>
     <row r="14">
@@ -1268,7 +1268,7 @@
         <v>0.00455240045961079</v>
       </c>
       <c r="T14" t="n">
-        <v>-0.0179937388482054</v>
+        <v>-0.0188074646708687</v>
       </c>
     </row>
     <row r="15">
@@ -1330,7 +1330,7 @@
         <v>0.00233847014267316</v>
       </c>
       <c r="T15" t="n">
-        <v>0.0276292582147641</v>
+        <v>0.0179413638887479</v>
       </c>
     </row>
     <row r="16">
@@ -1392,7 +1392,7 @@
         <v>0.00109032845217988</v>
       </c>
       <c r="T16" t="n">
-        <v>0.0197943510483599</v>
+        <v>0.0183417598159164</v>
       </c>
     </row>
     <row r="17">
@@ -1454,7 +1454,7 @@
         <v>0.0179464862953829</v>
       </c>
       <c r="T17" t="n">
-        <v>-0.0426506428566784</v>
+        <v>-0.0403656367671708</v>
       </c>
     </row>
     <row r="18">
@@ -1516,7 +1516,7 @@
         <v>0.228611505321296</v>
       </c>
       <c r="T18" t="n">
-        <v>-0.000932168280232888</v>
+        <v>-0.0038444135005433</v>
       </c>
     </row>
     <row r="19">
@@ -1578,7 +1578,7 @@
         <v>0.00620459115425521</v>
       </c>
       <c r="T19" t="n">
-        <v>-0.0143321336842633</v>
+        <v>-0.0156289578168552</v>
       </c>
     </row>
     <row r="20">
@@ -1640,66 +1640,66 @@
         <v>1</v>
       </c>
       <c r="T20" t="n">
-        <v>0.0635166560920207</v>
+        <v>0.0620360195791417</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>0.0337525921132433</v>
+        <v>0.0287303267030508</v>
       </c>
       <c r="B21" t="n">
-        <v>-0.00102444424694228</v>
+        <v>-0.00495230430079656</v>
       </c>
       <c r="C21" t="n">
-        <v>0.0736324550142593</v>
+        <v>0.0678001612532612</v>
       </c>
       <c r="D21" t="n">
-        <v>-0.0493644672164725</v>
+        <v>-0.0467775591202038</v>
       </c>
       <c r="E21" t="n">
-        <v>-0.0411602433657146</v>
+        <v>-0.0391769925902026</v>
       </c>
       <c r="F21" t="n">
-        <v>-0.121544158018929</v>
+        <v>-0.120653422087976</v>
       </c>
       <c r="G21" t="n">
-        <v>0.112519738309319</v>
+        <v>0.11449442715349</v>
       </c>
       <c r="H21" t="n">
-        <v>0.0283522521926804</v>
+        <v>0.030974312496068</v>
       </c>
       <c r="I21" t="n">
-        <v>0.0552313760906616</v>
+        <v>0.0616668743602804</v>
       </c>
       <c r="J21" t="n">
-        <v>-0.0360267154150473</v>
+        <v>-0.0260576414308473</v>
       </c>
       <c r="K21" t="n">
-        <v>0.0182946147753705</v>
+        <v>0.0185889501276473</v>
       </c>
       <c r="L21" t="n">
-        <v>0.0206824311319558</v>
+        <v>0.0205364503277865</v>
       </c>
       <c r="M21" t="n">
-        <v>-0.0179937388482054</v>
+        <v>-0.0188074646708687</v>
       </c>
       <c r="N21" t="n">
-        <v>0.0276292582147641</v>
+        <v>0.0179413638887479</v>
       </c>
       <c r="O21" t="n">
-        <v>0.0197943510483599</v>
+        <v>0.0183417598159164</v>
       </c>
       <c r="P21" t="n">
-        <v>-0.0426506428566784</v>
+        <v>-0.0403656367671708</v>
       </c>
       <c r="Q21" t="n">
-        <v>-0.000932168280232888</v>
+        <v>-0.0038444135005433</v>
       </c>
       <c r="R21" t="n">
-        <v>-0.0143321336842633</v>
+        <v>-0.0156289578168552</v>
       </c>
       <c r="S21" t="n">
-        <v>0.0635166560920207</v>
+        <v>0.0620360195791417</v>
       </c>
       <c r="T21" t="n">
         <v>1</v>

</xml_diff>

<commit_message>
:up: att 2024.02.01 14:20
</commit_message>
<xml_diff>
--- a/correlacao.xlsx
+++ b/correlacao.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\files\projects\programacao\python\acoes_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85127E43-821E-48F5-9184-5BACAD504817}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1317245B-0014-4A38-B3F1-BCAB1D636466}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="26">
   <si>
     <t>L.P</t>
   </si>
@@ -99,15 +99,12 @@
   <si>
     <t>Div.Bruta.Patrimonio</t>
   </si>
-  <si>
-    <t>v_price</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -115,31 +112,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C5700"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="4">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -151,40 +130,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Neutro" xfId="1" builtinId="28"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -476,18 +431,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AB28"/>
+  <dimension ref="A1:AA27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="R25" sqref="R25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="22.42578125" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -566,2339 +518,2176 @@
       <c r="AA1" t="s">
         <v>25</v>
       </c>
-      <c r="AB1" t="s">
-        <v>26</v>
-      </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2">
         <v>1</v>
       </c>
       <c r="C2">
-        <v>0.76461893260872804</v>
+        <v>0.77019548445311603</v>
       </c>
       <c r="D2">
-        <v>0.74544169759985901</v>
+        <v>0.74759359239684098</v>
       </c>
       <c r="E2">
-        <v>0.32268306134757602</v>
+        <v>0.340937712895446</v>
       </c>
       <c r="F2">
-        <v>0.32299917904943698</v>
+        <v>0.34101210618295802</v>
       </c>
       <c r="G2">
-        <v>-3.08643114626477E-2</v>
+        <v>-4.4562478412324399E-2</v>
       </c>
       <c r="H2">
-        <v>-0.31558235893518999</v>
+        <v>-0.34137708618060902</v>
       </c>
       <c r="I2">
-        <v>-0.57901713355034701</v>
+        <v>-0.56404640123267502</v>
       </c>
       <c r="J2">
-        <v>-0.53965484311949896</v>
+        <v>-0.53781040383409595</v>
       </c>
       <c r="K2">
-        <v>-0.21416029245083601</v>
+        <v>-0.21468104320857201</v>
       </c>
       <c r="L2">
-        <v>-3.14479787020535E-3</v>
+        <v>-2.5181635045528499E-3</v>
       </c>
       <c r="M2">
-        <v>-4.4730479313802403E-3</v>
+        <v>-4.45078817333235E-3</v>
       </c>
       <c r="N2">
-        <v>2.7516933516524501E-2</v>
+        <v>2.81066609689158E-2</v>
       </c>
       <c r="O2">
-        <v>0.217422323038622</v>
+        <v>0.20416425963804699</v>
       </c>
       <c r="P2">
-        <v>3.3094956938273898E-2</v>
+        <v>2.7144847066243899E-2</v>
       </c>
       <c r="Q2">
-        <v>7.6476849551984596E-2</v>
+        <v>7.9318725520844999E-2</v>
       </c>
       <c r="R2">
-        <v>-5.0533929531747401E-2</v>
+        <v>-8.2267465207382495E-3</v>
       </c>
       <c r="S2">
-        <v>0.192340741480129</v>
+        <v>0.229596899130526</v>
       </c>
       <c r="T2">
-        <v>9.7633047198213405E-2</v>
+        <v>9.3381194751659097E-2</v>
       </c>
       <c r="U2">
-        <v>-0.27427194530577698</v>
+        <v>-0.23121821050775701</v>
       </c>
       <c r="V2">
-        <v>-0.31246448601912002</v>
+        <v>-0.27567437110297899</v>
       </c>
       <c r="W2">
-        <v>0.30871660314744298</v>
+        <v>0.28271681668785598</v>
       </c>
       <c r="X2">
-        <v>0.106218466727422</v>
+        <v>0.11166170546317</v>
       </c>
       <c r="Y2">
-        <v>0.12832966716114799</v>
+        <v>0.11105253485494</v>
       </c>
       <c r="Z2">
-        <v>1.36591290329088E-2</v>
+        <v>7.2011969225451696E-3</v>
       </c>
       <c r="AA2">
-        <v>0.299847992281363</v>
-      </c>
-      <c r="AB2">
-        <v>0.11551680549042501</v>
+        <v>0.31383614451548902</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3">
-        <v>0.76461893260872804</v>
+        <v>0.77019548445311603</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3">
-        <v>0.87666286667849203</v>
+        <v>0.87929832346876402</v>
       </c>
       <c r="E3">
-        <v>0.36696984122932302</v>
+        <v>0.374802830273335</v>
       </c>
       <c r="F3">
-        <v>0.36752410428320098</v>
+        <v>0.37533559190708898</v>
       </c>
       <c r="G3">
-        <v>4.4120895065961403E-2</v>
+        <v>5.2995624609244098E-2</v>
       </c>
       <c r="H3">
-        <v>-0.118701113131329</v>
+        <v>-0.124965959032936</v>
       </c>
       <c r="I3">
-        <v>-0.32441172653840999</v>
+        <v>-0.31810525750665902</v>
       </c>
       <c r="J3">
-        <v>-0.756901293562386</v>
+        <v>-0.75571840098701504</v>
       </c>
       <c r="K3">
-        <v>-0.284636576961867</v>
+        <v>-0.27770002153364998</v>
       </c>
       <c r="L3">
-        <v>-2.3675652993991399E-4</v>
+        <v>8.7473746690606502E-5</v>
       </c>
       <c r="M3">
-        <v>-1.7893390114409E-4</v>
+        <v>5.9830228982908705E-4</v>
       </c>
       <c r="N3">
-        <v>3.0465562004755999E-2</v>
+        <v>3.05890661000809E-2</v>
       </c>
       <c r="O3">
-        <v>0.33374957905164399</v>
+        <v>0.31451135648442802</v>
       </c>
       <c r="P3">
-        <v>1.2113916385485E-2</v>
+        <v>2.76209049500623E-3</v>
       </c>
       <c r="Q3">
-        <v>6.1758621770236499E-2</v>
+        <v>6.6703492018527599E-2</v>
       </c>
       <c r="R3">
-        <v>0.34914727967808801</v>
+        <v>0.40685232574842101</v>
       </c>
       <c r="S3">
-        <v>0.61645101991369999</v>
+        <v>0.657939912070587</v>
       </c>
       <c r="T3">
-        <v>9.2004902025702301E-3</v>
+        <v>9.2287791105834498E-3</v>
       </c>
       <c r="U3">
-        <v>-0.14680572573886</v>
+        <v>-0.149649136160553</v>
       </c>
       <c r="V3">
-        <v>-0.166649416939254</v>
+        <v>-0.173611531697661</v>
       </c>
       <c r="W3">
-        <v>0.25145428235935702</v>
+        <v>0.242517664830741</v>
       </c>
       <c r="X3">
-        <v>0.184360914792182</v>
+        <v>0.184808441212753</v>
       </c>
       <c r="Y3">
-        <v>0.105867381114794</v>
+        <v>0.10656092611986399</v>
       </c>
       <c r="Z3">
-        <v>7.9201619499369505E-2</v>
+        <v>8.3620463458723399E-2</v>
       </c>
       <c r="AA3">
-        <v>0.33142437400341002</v>
-      </c>
-      <c r="AB3">
-        <v>8.8196514222277797E-2</v>
+        <v>0.33746400655331199</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4">
-        <v>0.74544169759985901</v>
+        <v>0.74759359239684098</v>
       </c>
       <c r="C4">
-        <v>0.87666286667849203</v>
+        <v>0.87929832346876402</v>
       </c>
       <c r="D4">
         <v>1</v>
       </c>
       <c r="E4">
-        <v>5.4519282030661498E-3</v>
+        <v>5.2937979187895499E-3</v>
       </c>
       <c r="F4">
-        <v>5.7267907470721201E-3</v>
+        <v>5.5099653634893796E-3</v>
       </c>
       <c r="G4">
-        <v>3.1150943518930999E-2</v>
+        <v>3.8306961768073799E-2</v>
       </c>
       <c r="H4">
-        <v>-0.228774028231959</v>
+        <v>-0.25099154185153999</v>
       </c>
       <c r="I4">
-        <v>-0.45823222893103699</v>
+        <v>-0.43812361788167598</v>
       </c>
       <c r="J4">
-        <v>-0.90052202864047903</v>
+        <v>-0.89876247869572801</v>
       </c>
       <c r="K4">
-        <v>-0.34375959034472697</v>
+        <v>-0.33815909601198701</v>
       </c>
       <c r="L4">
-        <v>-3.8139118903252698E-3</v>
+        <v>-3.1479029122296002E-3</v>
       </c>
       <c r="M4">
-        <v>-4.7123774164110899E-3</v>
+        <v>-5.0513728878800396E-3</v>
       </c>
       <c r="N4">
-        <v>3.0618489972592099E-2</v>
+        <v>3.0571080329957201E-2</v>
       </c>
       <c r="O4">
-        <v>0.27481481532714103</v>
+        <v>0.25594233862455501</v>
       </c>
       <c r="P4">
-        <v>9.6371787268209608E-3</v>
+        <v>6.8582345382799904E-3</v>
       </c>
       <c r="Q4">
-        <v>7.66935286386832E-2</v>
+        <v>8.0452219366215494E-2</v>
       </c>
       <c r="R4">
-        <v>0.50715499005045905</v>
+        <v>0.54909709484259595</v>
       </c>
       <c r="S4">
-        <v>0.68613351220254604</v>
+        <v>0.73076156845948304</v>
       </c>
       <c r="T4">
-        <v>1.8525892176001001E-2</v>
+        <v>1.7468997559584799E-2</v>
       </c>
       <c r="U4">
-        <v>-0.274135584536364</v>
+        <v>-0.244802331775438</v>
       </c>
       <c r="V4">
-        <v>-0.29579747228888198</v>
+        <v>-0.27149010189258199</v>
       </c>
       <c r="W4">
-        <v>0.29351299034254902</v>
+        <v>0.30235439958153498</v>
       </c>
       <c r="X4">
-        <v>0.155435978090565</v>
+        <v>0.15895178470000801</v>
       </c>
       <c r="Y4">
-        <v>9.87840398923166E-2</v>
+        <v>0.10148969151331</v>
       </c>
       <c r="Z4">
-        <v>7.7058195484517797E-2</v>
+        <v>8.1089629525839604E-2</v>
       </c>
       <c r="AA4">
-        <v>2.88586097253971E-2</v>
-      </c>
-      <c r="AB4">
-        <v>4.1587117080718501E-2</v>
+        <v>2.8091186266488499E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5">
-        <v>0.32268306134757602</v>
+        <v>0.340937712895446</v>
       </c>
       <c r="C5">
-        <v>0.36696984122932302</v>
+        <v>0.374802830273335</v>
       </c>
       <c r="D5">
-        <v>5.4519282030661498E-3</v>
+        <v>5.2937979187895499E-3</v>
       </c>
       <c r="E5">
         <v>1</v>
       </c>
       <c r="F5">
-        <v>0.99830259226227502</v>
+        <v>0.998302427897091</v>
       </c>
       <c r="G5">
-        <v>-3.9250889755323296E-3</v>
+        <v>-3.9281639410288097E-3</v>
       </c>
       <c r="H5">
-        <v>8.15256494993091E-2</v>
+        <v>9.0756654812176193E-2</v>
       </c>
       <c r="I5">
-        <v>7.5310693970542103E-2</v>
+        <v>7.7523800962662398E-2</v>
       </c>
       <c r="J5">
-        <v>9.7948847452346402E-2</v>
+        <v>0.101335834529446</v>
       </c>
       <c r="K5">
-        <v>-7.1268271791046899E-3</v>
+        <v>-7.0494559369220604E-3</v>
       </c>
       <c r="L5">
-        <v>7.6367794501457401E-4</v>
+        <v>7.8044664335213596E-4</v>
       </c>
       <c r="M5">
-        <v>-1.44056043030611E-3</v>
+        <v>-1.1763265795121801E-3</v>
       </c>
       <c r="N5">
-        <v>5.0427230206229602E-4</v>
+        <v>5.11597179451183E-4</v>
       </c>
       <c r="O5">
-        <v>8.9273331418443597E-2</v>
+        <v>8.5128203813558206E-2</v>
       </c>
       <c r="P5">
-        <v>-4.8184877740187801E-2</v>
+        <v>-4.78023951215081E-2</v>
       </c>
       <c r="Q5">
-        <v>-3.0711712386999102E-2</v>
+        <v>-3.2053466194342198E-2</v>
       </c>
       <c r="R5">
-        <v>-0.24974672937193401</v>
+        <v>-0.26904441908429499</v>
       </c>
       <c r="S5">
-        <v>-0.166807040029047</v>
+        <v>-0.16901237624464299</v>
       </c>
       <c r="T5">
-        <v>-3.8286059098724201E-3</v>
+        <v>-3.7944865833659902E-3</v>
       </c>
       <c r="U5">
-        <v>6.9601065794114694E-2</v>
+        <v>8.0007392848681094E-2</v>
       </c>
       <c r="V5">
-        <v>3.2065359025625399E-2</v>
+        <v>3.9620112766821397E-2</v>
       </c>
       <c r="W5">
-        <v>-0.29217114663811</v>
+        <v>-0.291260818856867</v>
       </c>
       <c r="X5">
-        <v>-9.7928991955129496E-2</v>
+        <v>-9.7555328419099696E-2</v>
       </c>
       <c r="Y5">
-        <v>-7.5401385422106906E-2</v>
+        <v>-7.4931641304289906E-2</v>
       </c>
       <c r="Z5">
-        <v>-9.2943492465488803E-2</v>
+        <v>-9.1718760780692202E-2</v>
       </c>
       <c r="AA5">
-        <v>0.85174328645703801</v>
-      </c>
-      <c r="AB5">
-        <v>0.12916707422576201</v>
+        <v>0.85170465942389495</v>
       </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6">
-        <v>0.32299917904943698</v>
+        <v>0.34101210618295802</v>
       </c>
       <c r="C6">
-        <v>0.36752410428320098</v>
+        <v>0.37533559190708898</v>
       </c>
       <c r="D6">
-        <v>5.7267907470721201E-3</v>
+        <v>5.5099653634893796E-3</v>
       </c>
       <c r="E6">
-        <v>0.99830259226227502</v>
+        <v>0.998302427897091</v>
       </c>
       <c r="F6">
         <v>1</v>
       </c>
       <c r="G6">
-        <v>-5.1525006057021499E-3</v>
+        <v>-5.1554827753487204E-3</v>
       </c>
       <c r="H6">
-        <v>7.8947593739114294E-2</v>
+        <v>8.8199229427284601E-2</v>
       </c>
       <c r="I6">
-        <v>7.3809906351473997E-2</v>
+        <v>7.60762798671209E-2</v>
       </c>
       <c r="J6">
-        <v>9.7077176622932193E-2</v>
+        <v>0.100507108469765</v>
       </c>
       <c r="K6">
-        <v>-7.4044725505608196E-3</v>
+        <v>-7.3177336662995102E-3</v>
       </c>
       <c r="L6">
-        <v>8.6932140492186497E-4</v>
+        <v>8.8864380932635598E-4</v>
       </c>
       <c r="M6">
-        <v>-1.3437701750363799E-3</v>
+        <v>-1.04548239404778E-3</v>
       </c>
       <c r="N6">
-        <v>2.5768142854550699E-3</v>
+        <v>2.5841625738847098E-3</v>
       </c>
       <c r="O6">
-        <v>8.9753725966218098E-2</v>
+        <v>8.5715672838614101E-2</v>
       </c>
       <c r="P6">
-        <v>-4.4649673829925601E-2</v>
+        <v>-4.4251840313347897E-2</v>
       </c>
       <c r="Q6">
-        <v>-3.1138286360568101E-2</v>
+        <v>-3.3380394072347302E-2</v>
       </c>
       <c r="R6">
-        <v>-0.253585572966739</v>
+        <v>-0.27284452822077099</v>
       </c>
       <c r="S6">
-        <v>-0.16652478165910101</v>
+        <v>-0.16917322408693</v>
       </c>
       <c r="T6">
-        <v>-2.6353242269411001E-3</v>
+        <v>-2.5975808222926098E-3</v>
       </c>
       <c r="U6">
-        <v>6.6575436053175605E-2</v>
+        <v>7.6869614355027496E-2</v>
       </c>
       <c r="V6">
-        <v>2.88335492437807E-2</v>
+        <v>3.6206859110848803E-2</v>
       </c>
       <c r="W6">
-        <v>-0.29512104598598898</v>
+        <v>-0.29421982112524397</v>
       </c>
       <c r="X6">
-        <v>-0.10377720036309</v>
+        <v>-0.103382911920406</v>
       </c>
       <c r="Y6">
-        <v>-8.1589034518109296E-2</v>
+        <v>-8.1019166564176806E-2</v>
       </c>
       <c r="Z6">
-        <v>-9.8770921338221504E-2</v>
+        <v>-9.7546844149951906E-2</v>
       </c>
       <c r="AA6">
-        <v>0.85541237804162695</v>
-      </c>
-      <c r="AB6">
-        <v>0.132520881323752</v>
+        <v>0.85537912146148098</v>
       </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
       <c r="B7">
-        <v>-3.08643114626477E-2</v>
+        <v>-4.4562478412324399E-2</v>
       </c>
       <c r="C7">
-        <v>4.4120895065961403E-2</v>
+        <v>5.2995624609244098E-2</v>
       </c>
       <c r="D7">
-        <v>3.1150943518930999E-2</v>
+        <v>3.8306961768073799E-2</v>
       </c>
       <c r="E7">
-        <v>-3.9250889755323296E-3</v>
+        <v>-3.9281639410288097E-3</v>
       </c>
       <c r="F7">
-        <v>-5.1525006057021499E-3</v>
+        <v>-5.1554827753487204E-3</v>
       </c>
       <c r="G7">
         <v>1</v>
       </c>
       <c r="H7">
-        <v>5.2963562599220903E-3</v>
+        <v>4.3794430581481497E-3</v>
       </c>
       <c r="I7">
-        <v>-9.0539665072304296E-3</v>
+        <v>-1.37563689076769E-2</v>
       </c>
       <c r="J7">
-        <v>-5.9728668283434497E-3</v>
+        <v>-9.4616924190091302E-3</v>
       </c>
       <c r="K7">
-        <v>-6.1404000758273597E-2</v>
+        <v>-6.1396237221348703E-2</v>
       </c>
       <c r="L7">
-        <v>3.08525979478898E-2</v>
+        <v>3.0922317761045499E-2</v>
       </c>
       <c r="M7">
-        <v>3.4202640862191401E-2</v>
+        <v>3.44597811164125E-2</v>
       </c>
       <c r="N7">
-        <v>-2.7412405880926998E-3</v>
+        <v>-2.7557380120292602E-3</v>
       </c>
       <c r="O7">
-        <v>3.7273258117419703E-2</v>
+        <v>3.65356599773278E-2</v>
       </c>
       <c r="P7">
-        <v>8.0532550059613794E-2</v>
+        <v>8.0556735425868095E-2</v>
       </c>
       <c r="Q7">
-        <v>6.2768745720168106E-2</v>
+        <v>7.0163574030509906E-2</v>
       </c>
       <c r="R7">
-        <v>9.4932267765649406E-2</v>
+        <v>0.134074604730446</v>
       </c>
       <c r="S7">
-        <v>-5.1605625587822397E-2</v>
+        <v>-6.2731100353620103E-2</v>
       </c>
       <c r="T7">
-        <v>7.06203816190909E-3</v>
+        <v>7.0548692528608703E-3</v>
       </c>
       <c r="U7">
-        <v>-1.64518954950152E-2</v>
+        <v>-3.1698002323982101E-2</v>
       </c>
       <c r="V7">
-        <v>6.4456573214850604E-3</v>
+        <v>-5.5766781916063404E-4</v>
       </c>
       <c r="W7">
-        <v>0.29318972577584301</v>
+        <v>0.341083700157509</v>
       </c>
       <c r="X7">
-        <v>0.113515540492533</v>
+        <v>0.11358951710111399</v>
       </c>
       <c r="Y7">
-        <v>0.630997245905774</v>
+        <v>0.63066920458550302</v>
       </c>
       <c r="Z7">
-        <v>0.44292299487454401</v>
+        <v>0.44828804845697201</v>
       </c>
       <c r="AA7">
-        <v>9.7514178750354192E-3</v>
-      </c>
-      <c r="AB7">
-        <v>9.8158634808821102E-2</v>
+        <v>9.8020220511193593E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
       <c r="B8">
-        <v>-0.31558235893518999</v>
+        <v>-0.34137708618060902</v>
       </c>
       <c r="C8">
-        <v>-0.118701113131329</v>
+        <v>-0.124965959032936</v>
       </c>
       <c r="D8">
-        <v>-0.228774028231959</v>
+        <v>-0.25099154185153999</v>
       </c>
       <c r="E8">
-        <v>8.15256494993091E-2</v>
+        <v>9.0756654812176193E-2</v>
       </c>
       <c r="F8">
-        <v>7.8947593739114294E-2</v>
+        <v>8.8199229427284601E-2</v>
       </c>
       <c r="G8">
-        <v>5.2963562599220903E-3</v>
+        <v>4.3794430581481497E-3</v>
       </c>
       <c r="H8">
         <v>1</v>
       </c>
       <c r="I8">
-        <v>0.54942009469747799</v>
+        <v>0.55252799745384396</v>
       </c>
       <c r="J8">
-        <v>0.27734960743814002</v>
+        <v>0.29294974213120001</v>
       </c>
       <c r="K8">
-        <v>-8.7359346047913997E-2</v>
+        <v>-8.3482341300325294E-2</v>
       </c>
       <c r="L8">
-        <v>-0.22559137934925699</v>
+        <v>-0.192750978830213</v>
       </c>
       <c r="M8">
-        <v>-0.22070019994412499</v>
+        <v>-0.18543231995436399</v>
       </c>
       <c r="N8">
-        <v>-2.8235141871421301E-2</v>
+        <v>-2.94292338174214E-2</v>
       </c>
       <c r="O8">
-        <v>6.6178359887472907E-2</v>
+        <v>6.0382590982233697E-2</v>
       </c>
       <c r="P8">
-        <v>-7.7167067019687799E-2</v>
+        <v>-7.9817478782015006E-2</v>
       </c>
       <c r="Q8">
-        <v>1.91391852091212E-3</v>
+        <v>3.1646720319864299E-4</v>
       </c>
       <c r="R8">
-        <v>9.2003553668667207E-2</v>
+        <v>7.7385334669495098E-2</v>
       </c>
       <c r="S8">
-        <v>-1.33711823739062E-2</v>
+        <v>-1.2467707776255501E-2</v>
       </c>
       <c r="T8">
-        <v>0.118098410497816</v>
+        <v>0.11276700276788799</v>
       </c>
       <c r="U8">
-        <v>0.254847393876033</v>
+        <v>0.26114151985933198</v>
       </c>
       <c r="V8">
-        <v>0.26044746788297701</v>
+        <v>0.27050690871508298</v>
       </c>
       <c r="W8">
-        <v>-0.127480137885496</v>
+        <v>-0.115392950843674</v>
       </c>
       <c r="X8">
-        <v>-4.4181101265618999E-2</v>
+        <v>-4.5229299345927003E-2</v>
       </c>
       <c r="Y8">
-        <v>-0.17978042859919199</v>
+        <v>-0.175414737082462</v>
       </c>
       <c r="Z8">
-        <v>-0.16203001598061501</v>
+        <v>-0.162096064853503</v>
       </c>
       <c r="AA8">
-        <v>0.119790809929619</v>
-      </c>
-      <c r="AB8">
-        <v>2.2949054905322602E-2</v>
+        <v>0.12558832479895801</v>
       </c>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
       <c r="B9">
-        <v>-0.57901713355034701</v>
+        <v>-0.56404640123267502</v>
       </c>
       <c r="C9">
-        <v>-0.32441172653840999</v>
+        <v>-0.31810525750665902</v>
       </c>
       <c r="D9">
-        <v>-0.45823222893103699</v>
+        <v>-0.43812361788167598</v>
       </c>
       <c r="E9">
-        <v>7.5310693970542103E-2</v>
+        <v>7.7523800962662398E-2</v>
       </c>
       <c r="F9">
-        <v>7.3809906351473997E-2</v>
+        <v>7.60762798671209E-2</v>
       </c>
       <c r="G9">
-        <v>-9.0539665072304296E-3</v>
+        <v>-1.37563689076769E-2</v>
       </c>
       <c r="H9">
-        <v>0.54942009469747799</v>
+        <v>0.55252799745384396</v>
       </c>
       <c r="I9">
         <v>1</v>
       </c>
       <c r="J9">
-        <v>0.43908756444188102</v>
+        <v>0.43633265643390301</v>
       </c>
       <c r="K9">
-        <v>0.15593282237403999</v>
+        <v>0.15596625737746</v>
       </c>
       <c r="L9">
-        <v>-1.7105209479905001E-2</v>
+        <v>-1.1914511859626199E-2</v>
       </c>
       <c r="M9">
-        <v>-1.56719745125391E-2</v>
+        <v>-9.4998504353443498E-3</v>
       </c>
       <c r="N9">
-        <v>-3.4004666239122502E-2</v>
+        <v>-3.2884229876801098E-2</v>
       </c>
       <c r="O9">
-        <v>-3.4283656622306799E-2</v>
+        <v>-2.8101733225975301E-2</v>
       </c>
       <c r="P9">
-        <v>-5.9065744121403002E-2</v>
+        <v>-6.2268065461786697E-2</v>
       </c>
       <c r="Q9">
-        <v>-0.105743228850102</v>
+        <v>-0.110808179370208</v>
       </c>
       <c r="R9">
-        <v>1.2485188650434499E-2</v>
+        <v>-3.8112614309388199E-2</v>
       </c>
       <c r="S9">
-        <v>-1.51747032953414E-2</v>
+        <v>-3.2254653599315099E-2</v>
       </c>
       <c r="T9">
-        <v>3.1531692662043601E-2</v>
+        <v>2.7123037488918401E-2</v>
       </c>
       <c r="U9">
-        <v>0.53765202284186298</v>
+        <v>0.56366019776934995</v>
       </c>
       <c r="V9">
-        <v>0.54644713348316998</v>
+        <v>0.57243081326907996</v>
       </c>
       <c r="W9">
-        <v>-0.43828925683601899</v>
+        <v>-0.498382560235619</v>
       </c>
       <c r="X9">
-        <v>-0.15803083212854099</v>
+        <v>-0.18216489085138801</v>
       </c>
       <c r="Y9">
-        <v>-0.20103723869006701</v>
+        <v>-0.20290023437662</v>
       </c>
       <c r="Z9">
-        <v>-0.17282585702009701</v>
+        <v>-0.18226350128587601</v>
       </c>
       <c r="AA9">
-        <v>4.9381628659003703E-2</v>
-      </c>
-      <c r="AB9">
-        <v>-9.2807682270836397E-2</v>
+        <v>5.3259383009840899E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
       <c r="B10">
-        <v>-0.53965484311949896</v>
+        <v>-0.53781040383409595</v>
       </c>
       <c r="C10">
-        <v>-0.756901293562386</v>
+        <v>-0.75571840098701504</v>
       </c>
       <c r="D10">
-        <v>-0.90052202864047903</v>
+        <v>-0.89876247869572801</v>
       </c>
       <c r="E10">
-        <v>9.7948847452346402E-2</v>
+        <v>0.101335834529446</v>
       </c>
       <c r="F10">
-        <v>9.7077176622932193E-2</v>
+        <v>0.100507108469765</v>
       </c>
       <c r="G10">
-        <v>-5.9728668283434497E-3</v>
+        <v>-9.4616924190091302E-3</v>
       </c>
       <c r="H10">
-        <v>0.27734960743814002</v>
+        <v>0.29294974213120001</v>
       </c>
       <c r="I10">
-        <v>0.43908756444188102</v>
+        <v>0.43633265643390301</v>
       </c>
       <c r="J10">
         <v>1</v>
       </c>
       <c r="K10">
-        <v>0.39383800659956397</v>
+        <v>0.38501826036916398</v>
       </c>
       <c r="L10">
-        <v>-4.4889783977884803E-3</v>
+        <v>-2.24898391163881E-3</v>
       </c>
       <c r="M10">
-        <v>-5.0654054309602903E-3</v>
+        <v>-2.9874977496354002E-3</v>
       </c>
       <c r="N10">
-        <v>-3.87259904097896E-2</v>
+        <v>-3.8008191290301502E-2</v>
       </c>
       <c r="O10">
-        <v>-0.26004908871657301</v>
+        <v>-0.24549951176521401</v>
       </c>
       <c r="P10">
-        <v>-1.72882062719126E-2</v>
+        <v>-2.3902770457069601E-2</v>
       </c>
       <c r="Q10">
-        <v>-9.4212323686870394E-2</v>
+        <v>-0.101980284068711</v>
       </c>
       <c r="R10">
-        <v>-0.62016680878025798</v>
+        <v>-0.67066598121390097</v>
       </c>
       <c r="S10">
-        <v>-0.74197877818566005</v>
+        <v>-0.78979596181029998</v>
       </c>
       <c r="T10">
-        <v>-5.1377631770755904E-3</v>
+        <v>-6.6292066455728499E-3</v>
       </c>
       <c r="U10">
-        <v>0.40694226542013001</v>
+        <v>0.418908006946282</v>
       </c>
       <c r="V10">
-        <v>0.41422229936285998</v>
+        <v>0.43072012751969602</v>
       </c>
       <c r="W10">
-        <v>-0.30903094026378802</v>
+        <v>-0.32338621823109098</v>
       </c>
       <c r="X10">
-        <v>-0.137656247078076</v>
+        <v>-0.14711573401696201</v>
       </c>
       <c r="Y10">
-        <v>-0.143681301661506</v>
+        <v>-0.14620357332269901</v>
       </c>
       <c r="Z10">
-        <v>-0.125989281254833</v>
+        <v>-0.13545280154401099</v>
       </c>
       <c r="AA10">
-        <v>6.5826296400070705E-2</v>
-      </c>
-      <c r="AB10">
-        <v>-1.6418275480676401E-2</v>
+        <v>6.8718721527367202E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
       <c r="B11">
-        <v>-0.21416029245083601</v>
+        <v>-0.21468104320857201</v>
       </c>
       <c r="C11">
-        <v>-0.284636576961867</v>
+        <v>-0.27770002153364998</v>
       </c>
       <c r="D11">
-        <v>-0.34375959034472697</v>
+        <v>-0.33815909601198701</v>
       </c>
       <c r="E11">
-        <v>-7.1268271791046899E-3</v>
+        <v>-7.0494559369220604E-3</v>
       </c>
       <c r="F11">
-        <v>-7.4044725505608196E-3</v>
+        <v>-7.3177336662995102E-3</v>
       </c>
       <c r="G11">
-        <v>-6.1404000758273597E-2</v>
+        <v>-6.1396237221348703E-2</v>
       </c>
       <c r="H11">
-        <v>-8.7359346047913997E-2</v>
+        <v>-8.3482341300325294E-2</v>
       </c>
       <c r="I11">
-        <v>0.15593282237403999</v>
+        <v>0.15596625737746</v>
       </c>
       <c r="J11">
-        <v>0.39383800659956397</v>
+        <v>0.38501826036916398</v>
       </c>
       <c r="K11">
         <v>1</v>
       </c>
       <c r="L11">
-        <v>-1.2639430645690701E-2</v>
+        <v>-1.2585022960754101E-2</v>
       </c>
       <c r="M11">
-        <v>-2.2669081522146799E-2</v>
+        <v>-2.1862861669903901E-2</v>
       </c>
       <c r="N11">
-        <v>-7.83949144332097E-2</v>
+        <v>-7.8378454657876698E-2</v>
       </c>
       <c r="O11">
-        <v>-0.64966788460760205</v>
+        <v>-0.60917993036653795</v>
       </c>
       <c r="P11">
-        <v>-3.4446283324123597E-2</v>
+        <v>-3.3761615577036899E-2</v>
       </c>
       <c r="Q11">
-        <v>-8.4228448591064806E-2</v>
+        <v>-9.0686165248101094E-2</v>
       </c>
       <c r="R11">
-        <v>-0.227044055411766</v>
+        <v>-0.24618434179097901</v>
       </c>
       <c r="S11">
-        <v>-0.21253665298656299</v>
+        <v>-0.218524497327061</v>
       </c>
       <c r="T11">
-        <v>-1.36880537788284E-2</v>
+        <v>-1.36056608132861E-2</v>
       </c>
       <c r="U11">
-        <v>0.26245840079336002</v>
+        <v>0.281345371688493</v>
       </c>
       <c r="V11">
-        <v>0.24322096589928699</v>
+        <v>0.26817683671872</v>
       </c>
       <c r="W11">
-        <v>-0.123633509631869</v>
+        <v>-0.136202597322164</v>
       </c>
       <c r="X11">
-        <v>-0.112091492470516</v>
+        <v>-0.11019383218053699</v>
       </c>
       <c r="Y11">
-        <v>-0.122682584322403</v>
+        <v>-0.122316539374464</v>
       </c>
       <c r="Z11">
-        <v>-0.13458667157922799</v>
+        <v>-0.13340187259202699</v>
       </c>
       <c r="AA11">
-        <v>-3.1815122094351403E-2</v>
-      </c>
-      <c r="AB11">
-        <v>-7.6688667774808802E-2</v>
+        <v>-3.1673041878570299E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
       <c r="B12">
-        <v>-3.14479787020535E-3</v>
+        <v>-2.5181635045528499E-3</v>
       </c>
       <c r="C12">
-        <v>-2.3675652993991399E-4</v>
+        <v>8.7473746690606502E-5</v>
       </c>
       <c r="D12">
-        <v>-3.8139118903252698E-3</v>
+        <v>-3.1479029122296002E-3</v>
       </c>
       <c r="E12">
-        <v>7.6367794501457401E-4</v>
+        <v>7.8044664335213596E-4</v>
       </c>
       <c r="F12">
-        <v>8.6932140492186497E-4</v>
+        <v>8.8864380932635598E-4</v>
       </c>
       <c r="G12">
-        <v>3.08525979478898E-2</v>
+        <v>3.0922317761045499E-2</v>
       </c>
       <c r="H12">
-        <v>-0.22559137934925699</v>
+        <v>-0.192750978830213</v>
       </c>
       <c r="I12">
-        <v>-1.7105209479905001E-2</v>
+        <v>-1.1914511859626199E-2</v>
       </c>
       <c r="J12">
-        <v>-4.4889783977884803E-3</v>
+        <v>-2.24898391163881E-3</v>
       </c>
       <c r="K12">
-        <v>-1.2639430645690701E-2</v>
+        <v>-1.2585022960754101E-2</v>
       </c>
       <c r="L12">
         <v>1</v>
       </c>
       <c r="M12">
-        <v>0.99791334266167098</v>
+        <v>0.994906460022145</v>
       </c>
       <c r="N12">
-        <v>-3.7701204714295403E-2</v>
+        <v>-3.7718352222079102E-2</v>
       </c>
       <c r="O12">
-        <v>-0.16842943732311</v>
+        <v>-0.154083948603287</v>
       </c>
       <c r="P12">
-        <v>8.0129441134986698E-2</v>
+        <v>8.0872502731068094E-2</v>
       </c>
       <c r="Q12">
-        <v>-3.6393438971727102E-2</v>
+        <v>-3.5734433194290302E-2</v>
       </c>
       <c r="R12">
-        <v>4.7411123441410104E-3</v>
+        <v>5.2886502773233403E-3</v>
       </c>
       <c r="S12">
-        <v>2.2611843744352799E-3</v>
+        <v>1.5704901943191E-3</v>
       </c>
       <c r="T12">
-        <v>3.2323426782878799E-3</v>
+        <v>3.2421204109885399E-3</v>
       </c>
       <c r="U12">
-        <v>2.9355293171958501E-2</v>
+        <v>2.9959979199500199E-2</v>
       </c>
       <c r="V12">
-        <v>2.98324955844738E-2</v>
+        <v>3.0662008921144599E-2</v>
       </c>
       <c r="W12">
-        <v>0.119848063794434</v>
+        <v>0.10003270628434401</v>
       </c>
       <c r="X12">
-        <v>0.124677379081522</v>
+        <v>0.12506885368253401</v>
       </c>
       <c r="Y12">
-        <v>0.17232256502187901</v>
+        <v>0.17167983096360301</v>
       </c>
       <c r="Z12">
-        <v>0.155322282671887</v>
+        <v>0.15923748453613401</v>
       </c>
       <c r="AA12">
-        <v>8.7544496803485701E-3</v>
-      </c>
-      <c r="AB12">
-        <v>-4.1470834838146502E-2</v>
+        <v>8.8428071405106997E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>11</v>
       </c>
       <c r="B13">
-        <v>-4.4730479313802403E-3</v>
+        <v>-4.45078817333235E-3</v>
       </c>
       <c r="C13">
-        <v>-1.7893390114409E-4</v>
+        <v>5.9830228982908705E-4</v>
       </c>
       <c r="D13">
-        <v>-4.7123774164110899E-3</v>
+        <v>-5.0513728878800396E-3</v>
       </c>
       <c r="E13">
-        <v>-1.44056043030611E-3</v>
+        <v>-1.1763265795121801E-3</v>
       </c>
       <c r="F13">
-        <v>-1.3437701750363799E-3</v>
+        <v>-1.04548239404778E-3</v>
       </c>
       <c r="G13">
-        <v>3.4202640862191401E-2</v>
+        <v>3.44597811164125E-2</v>
       </c>
       <c r="H13">
-        <v>-0.22070019994412499</v>
+        <v>-0.18543231995436399</v>
       </c>
       <c r="I13">
-        <v>-1.56719745125391E-2</v>
+        <v>-9.4998504353443498E-3</v>
       </c>
       <c r="J13">
-        <v>-5.0654054309602903E-3</v>
+        <v>-2.9874977496354002E-3</v>
       </c>
       <c r="K13">
-        <v>-2.2669081522146799E-2</v>
+        <v>-2.1862861669903901E-2</v>
       </c>
       <c r="L13">
-        <v>0.99791334266167098</v>
+        <v>0.994906460022145</v>
       </c>
       <c r="M13">
         <v>1</v>
       </c>
       <c r="N13">
-        <v>-4.6499785722364399E-2</v>
+        <v>-4.6408661351132002E-2</v>
       </c>
       <c r="O13">
-        <v>-0.14163398677821401</v>
+        <v>-0.102290341299504</v>
       </c>
       <c r="P13">
-        <v>8.4122157414466797E-2</v>
+        <v>8.9969747696619404E-2</v>
       </c>
       <c r="Q13">
-        <v>-3.8637866967884099E-2</v>
+        <v>-3.1024476874182399E-2</v>
       </c>
       <c r="R13">
-        <v>3.1717427432512101E-3</v>
+        <v>4.0052583856845601E-3</v>
       </c>
       <c r="S13">
-        <v>1.6378972797373001E-3</v>
+        <v>1.1508149086765799E-4</v>
       </c>
       <c r="T13">
-        <v>1.48331205726915E-3</v>
+        <v>1.7049318855510301E-3</v>
       </c>
       <c r="U13">
-        <v>3.1009265741002399E-2</v>
+        <v>3.2838646312183299E-2</v>
       </c>
       <c r="V13">
-        <v>3.3516794185490202E-2</v>
+        <v>3.6695186468913898E-2</v>
       </c>
       <c r="W13">
-        <v>0.12367342803864199</v>
+        <v>0.10703612136876101</v>
       </c>
       <c r="X13">
-        <v>0.131961337303349</v>
+        <v>0.13655745890273999</v>
       </c>
       <c r="Y13">
-        <v>0.17946890170118099</v>
+        <v>0.18358869007858999</v>
       </c>
       <c r="Z13">
-        <v>0.16890930148582001</v>
+        <v>0.17732317970556299</v>
       </c>
       <c r="AA13">
-        <v>7.4864131025065301E-3</v>
-      </c>
-      <c r="AB13">
-        <v>-3.7070355116631197E-2</v>
+        <v>8.3261505149158609E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
       <c r="B14">
-        <v>2.7516933516524501E-2</v>
+        <v>2.81066609689158E-2</v>
       </c>
       <c r="C14">
-        <v>3.0465562004755999E-2</v>
+        <v>3.05890661000809E-2</v>
       </c>
       <c r="D14">
-        <v>3.0618489972592099E-2</v>
+        <v>3.0571080329957201E-2</v>
       </c>
       <c r="E14">
-        <v>5.0427230206229602E-4</v>
+        <v>5.11597179451183E-4</v>
       </c>
       <c r="F14">
-        <v>2.5768142854550699E-3</v>
+        <v>2.5841625738847098E-3</v>
       </c>
       <c r="G14">
-        <v>-2.7412405880926998E-3</v>
+        <v>-2.7557380120292602E-3</v>
       </c>
       <c r="H14">
-        <v>-2.8235141871421301E-2</v>
+        <v>-2.94292338174214E-2</v>
       </c>
       <c r="I14">
-        <v>-3.4004666239122502E-2</v>
+        <v>-3.2884229876801098E-2</v>
       </c>
       <c r="J14">
-        <v>-3.87259904097896E-2</v>
+        <v>-3.8008191290301502E-2</v>
       </c>
       <c r="K14">
-        <v>-7.83949144332097E-2</v>
+        <v>-7.8378454657876698E-2</v>
       </c>
       <c r="L14">
-        <v>-3.7701204714295403E-2</v>
+        <v>-3.7718352222079102E-2</v>
       </c>
       <c r="M14">
-        <v>-4.6499785722364399E-2</v>
+        <v>-4.6408661351132002E-2</v>
       </c>
       <c r="N14">
         <v>1</v>
       </c>
       <c r="O14">
-        <v>0.14329931199673601</v>
+        <v>0.134642972610856</v>
       </c>
       <c r="P14">
-        <v>-2.2584096170448899E-2</v>
+        <v>-2.25178491624578E-2</v>
       </c>
       <c r="Q14">
-        <v>0.49331174641417203</v>
+        <v>0.14624085099530701</v>
       </c>
       <c r="R14">
-        <v>-3.6403412700444601E-2</v>
+        <v>-4.7225116602863104E-3</v>
       </c>
       <c r="S14">
-        <v>1.64946348161116E-2</v>
+        <v>1.71174642466396E-2</v>
       </c>
       <c r="T14">
-        <v>-9.5759427022190603E-4</v>
+        <v>-9.4735211482512005E-4</v>
       </c>
       <c r="U14">
-        <v>-3.5319360740704103E-2</v>
+        <v>-3.5882027050311398E-2</v>
       </c>
       <c r="V14">
-        <v>-3.5503142737454203E-2</v>
+        <v>-3.66043570610717E-2</v>
       </c>
       <c r="W14">
-        <v>-9.8458776218714292E-4</v>
+        <v>8.0572116785610002E-4</v>
       </c>
       <c r="X14">
-        <v>-2.5815755942230598E-2</v>
+        <v>-2.6054096300289101E-2</v>
       </c>
       <c r="Y14">
-        <v>-3.0079770288262999E-2</v>
+        <v>-3.1347358791964201E-2</v>
       </c>
       <c r="Z14">
-        <v>-4.9360245560671298E-2</v>
+        <v>-3.98924976064313E-2</v>
       </c>
       <c r="AA14">
-        <v>-4.3183151290990297E-3</v>
-      </c>
-      <c r="AB14">
-        <v>6.8194287379843399E-2</v>
+        <v>-4.32360625889974E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>13</v>
       </c>
       <c r="B15">
-        <v>0.217422323038622</v>
+        <v>0.20416425963804699</v>
       </c>
       <c r="C15">
-        <v>0.33374957905164399</v>
+        <v>0.31451135648442802</v>
       </c>
       <c r="D15">
-        <v>0.27481481532714103</v>
+        <v>0.25594233862455501</v>
       </c>
       <c r="E15">
-        <v>8.9273331418443597E-2</v>
+        <v>8.5128203813558206E-2</v>
       </c>
       <c r="F15">
-        <v>8.9753725966218098E-2</v>
+        <v>8.5715672838614101E-2</v>
       </c>
       <c r="G15">
-        <v>3.7273258117419703E-2</v>
+        <v>3.65356599773278E-2</v>
       </c>
       <c r="H15">
-        <v>6.6178359887472907E-2</v>
+        <v>6.0382590982233697E-2</v>
       </c>
       <c r="I15">
-        <v>-3.4283656622306799E-2</v>
+        <v>-2.8101733225975301E-2</v>
       </c>
       <c r="J15">
-        <v>-0.26004908871657301</v>
+        <v>-0.24549951176521401</v>
       </c>
       <c r="K15">
-        <v>-0.64966788460760205</v>
+        <v>-0.60917993036653795</v>
       </c>
       <c r="L15">
-        <v>-0.16842943732311</v>
+        <v>-0.154083948603287</v>
       </c>
       <c r="M15">
-        <v>-0.14163398677821401</v>
+        <v>-0.102290341299504</v>
       </c>
       <c r="N15">
-        <v>0.14329931199673601</v>
+        <v>0.134642972610856</v>
       </c>
       <c r="O15">
         <v>1</v>
       </c>
       <c r="P15">
-        <v>4.3401956368791302E-2</v>
+        <v>6.4447658571627597E-2</v>
       </c>
       <c r="Q15">
-        <v>0.10220829460688</v>
+        <v>0.10091891755919701</v>
       </c>
       <c r="R15">
-        <v>0.11582708155129599</v>
+        <v>0.12533379539155201</v>
       </c>
       <c r="S15">
-        <v>0.229060892436624</v>
+        <v>0.22536653433276399</v>
       </c>
       <c r="T15">
-        <v>6.2911492307972296E-3</v>
+        <v>6.8507037955172403E-3</v>
       </c>
       <c r="U15">
-        <v>7.8297070303933701E-3</v>
+        <v>1.27605333965073E-2</v>
       </c>
       <c r="V15">
-        <v>9.6136207107205707E-3</v>
+        <v>1.8337739530291899E-2</v>
       </c>
       <c r="W15">
-        <v>0.112052903910382</v>
+        <v>0.11714739026446599</v>
       </c>
       <c r="X15">
-        <v>6.81021547542391E-2</v>
+        <v>8.3290003715019906E-2</v>
       </c>
       <c r="Y15">
-        <v>8.1964377171543895E-2</v>
+        <v>0.10137185199915801</v>
       </c>
       <c r="Z15">
-        <v>7.5961979969116702E-2</v>
+        <v>9.4992075329119796E-2</v>
       </c>
       <c r="AA15">
-        <v>8.9493459482607299E-2</v>
-      </c>
-      <c r="AB15">
-        <v>8.5031160932701896E-2</v>
+        <v>8.7647954435012804E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>14</v>
       </c>
       <c r="B16">
-        <v>3.3094956938273898E-2</v>
+        <v>2.7144847066243899E-2</v>
       </c>
       <c r="C16">
-        <v>1.2113916385485E-2</v>
+        <v>2.76209049500623E-3</v>
       </c>
       <c r="D16">
-        <v>9.6371787268209608E-3</v>
+        <v>6.8582345382799904E-3</v>
       </c>
       <c r="E16">
-        <v>-4.8184877740187801E-2</v>
+        <v>-4.78023951215081E-2</v>
       </c>
       <c r="F16">
-        <v>-4.4649673829925601E-2</v>
+        <v>-4.4251840313347897E-2</v>
       </c>
       <c r="G16">
-        <v>8.0532550059613794E-2</v>
+        <v>8.0556735425868095E-2</v>
       </c>
       <c r="H16">
-        <v>-7.7167067019687799E-2</v>
+        <v>-7.9817478782015006E-2</v>
       </c>
       <c r="I16">
-        <v>-5.9065744121403002E-2</v>
+        <v>-6.2268065461786697E-2</v>
       </c>
       <c r="J16">
-        <v>-1.72882062719126E-2</v>
+        <v>-2.3902770457069601E-2</v>
       </c>
       <c r="K16">
-        <v>-3.4446283324123597E-2</v>
+        <v>-3.3761615577036899E-2</v>
       </c>
       <c r="L16">
-        <v>8.0129441134986698E-2</v>
+        <v>8.0872502731068094E-2</v>
       </c>
       <c r="M16">
-        <v>8.4122157414466797E-2</v>
+        <v>8.9969747696619404E-2</v>
       </c>
       <c r="N16">
-        <v>-2.2584096170448899E-2</v>
+        <v>-2.25178491624578E-2</v>
       </c>
       <c r="O16">
-        <v>4.3401956368791302E-2</v>
+        <v>6.4447658571627597E-2</v>
       </c>
       <c r="P16">
         <v>1</v>
       </c>
       <c r="Q16">
-        <v>-7.80063818550078E-2</v>
+        <v>-7.7346560720481294E-2</v>
       </c>
       <c r="R16">
-        <v>-0.21405282598304201</v>
+        <v>-0.14093703403793001</v>
       </c>
       <c r="S16">
-        <v>0.24235115251148101</v>
+        <v>0.101271099925174</v>
       </c>
       <c r="T16">
-        <v>3.6756898156804302E-2</v>
+        <v>3.6889406369608101E-2</v>
       </c>
       <c r="U16">
-        <v>2.0003779542233001E-2</v>
+        <v>-1.1030756180542499E-3</v>
       </c>
       <c r="V16">
-        <v>1.9454694727210099E-2</v>
+        <v>-3.4873895181731598E-3</v>
       </c>
       <c r="W16">
-        <v>2.6518918379687201E-2</v>
+        <v>4.8663627356813698E-2</v>
       </c>
       <c r="X16">
-        <v>-1.6855431979829201E-2</v>
+        <v>-1.1529934233992701E-2</v>
       </c>
       <c r="Y16">
-        <v>9.7546108678770605E-3</v>
+        <v>1.4238887284318E-2</v>
       </c>
       <c r="Z16">
-        <v>1.10871733451552E-2</v>
+        <v>7.3159325252599499E-3</v>
       </c>
       <c r="AA16">
-        <v>-2.2041702572722099E-2</v>
-      </c>
-      <c r="AB16">
-        <v>3.2852948162221701E-2</v>
+        <v>-2.14679090719587E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>15</v>
       </c>
       <c r="B17">
-        <v>7.6476849551984596E-2</v>
+        <v>7.9318725520844999E-2</v>
       </c>
       <c r="C17">
-        <v>6.1758621770236499E-2</v>
+        <v>6.6703492018527599E-2</v>
       </c>
       <c r="D17">
-        <v>7.66935286386832E-2</v>
+        <v>8.0452219366215494E-2</v>
       </c>
       <c r="E17">
-        <v>-3.0711712386999102E-2</v>
+        <v>-3.2053466194342198E-2</v>
       </c>
       <c r="F17">
-        <v>-3.1138286360568101E-2</v>
+        <v>-3.3380394072347302E-2</v>
       </c>
       <c r="G17">
-        <v>6.2768745720168106E-2</v>
+        <v>7.0163574030509906E-2</v>
       </c>
       <c r="H17">
-        <v>1.91391852091212E-3</v>
+        <v>3.1646720319864299E-4</v>
       </c>
       <c r="I17">
-        <v>-0.105743228850102</v>
+        <v>-0.110808179370208</v>
       </c>
       <c r="J17">
-        <v>-9.4212323686870394E-2</v>
+        <v>-0.101980284068711</v>
       </c>
       <c r="K17">
-        <v>-8.4228448591064806E-2</v>
+        <v>-9.0686165248101094E-2</v>
       </c>
       <c r="L17">
-        <v>-3.6393438971727102E-2</v>
+        <v>-3.5734433194290302E-2</v>
       </c>
       <c r="M17">
-        <v>-3.8637866967884099E-2</v>
+        <v>-3.1024476874182399E-2</v>
       </c>
       <c r="N17">
-        <v>0.49331174641417203</v>
+        <v>0.14624085099530701</v>
       </c>
       <c r="O17">
-        <v>0.10220829460688</v>
+        <v>0.10091891755919701</v>
       </c>
       <c r="P17">
-        <v>-7.80063818550078E-2</v>
+        <v>-7.7346560720481294E-2</v>
       </c>
       <c r="Q17">
         <v>1</v>
       </c>
       <c r="R17">
-        <v>5.8168199099966997E-2</v>
+        <v>9.5647160959361197E-2</v>
       </c>
       <c r="S17">
-        <v>4.2076503206321801E-2</v>
+        <v>5.36573704086468E-2</v>
       </c>
       <c r="T17">
-        <v>7.0146639419401604E-3</v>
+        <v>9.8027315292476304E-3</v>
       </c>
       <c r="U17">
-        <v>-3.8606221400018403E-2</v>
+        <v>-4.7437735153015102E-2</v>
       </c>
       <c r="V17">
-        <v>-4.2131966352810697E-2</v>
+        <v>-5.0366191334870698E-2</v>
       </c>
       <c r="W17">
-        <v>0.120727511181492</v>
+        <v>0.13378126700394699</v>
       </c>
       <c r="X17">
-        <v>0.14632188638653101</v>
+        <v>0.168862769211928</v>
       </c>
       <c r="Y17">
-        <v>0.24637340129289301</v>
+        <v>0.287109185823404</v>
       </c>
       <c r="Z17">
-        <v>0.16572052342295501</v>
+        <v>0.20979604381692801</v>
       </c>
       <c r="AA17">
-        <v>1.79028107531937E-2</v>
-      </c>
-      <c r="AB17">
-        <v>0.18393054966036501</v>
+        <v>2.4902457039188301E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>16</v>
       </c>
       <c r="B18">
-        <v>-5.0533929531747401E-2</v>
+        <v>-8.2267465207382495E-3</v>
       </c>
       <c r="C18">
-        <v>0.34914727967808801</v>
+        <v>0.40685232574842101</v>
       </c>
       <c r="D18">
-        <v>0.50715499005045905</v>
+        <v>0.54909709484259595</v>
       </c>
       <c r="E18">
-        <v>-0.24974672937193401</v>
+        <v>-0.26904441908429499</v>
       </c>
       <c r="F18">
-        <v>-0.253585572966739</v>
+        <v>-0.27284452822077099</v>
       </c>
       <c r="G18">
-        <v>9.4932267765649406E-2</v>
+        <v>0.134074604730446</v>
       </c>
       <c r="H18">
-        <v>9.2003553668667207E-2</v>
+        <v>7.7385334669495098E-2</v>
       </c>
       <c r="I18">
-        <v>1.2485188650434499E-2</v>
+        <v>-3.8112614309388199E-2</v>
       </c>
       <c r="J18">
-        <v>-0.62016680878025798</v>
+        <v>-0.67066598121390097</v>
       </c>
       <c r="K18">
-        <v>-0.227044055411766</v>
+        <v>-0.24618434179097901</v>
       </c>
       <c r="L18">
-        <v>4.7411123441410104E-3</v>
+        <v>5.2886502773233403E-3</v>
       </c>
       <c r="M18">
-        <v>3.1717427432512101E-3</v>
+        <v>4.0052583856845601E-3</v>
       </c>
       <c r="N18">
-        <v>-3.6403412700444601E-2</v>
+        <v>-4.7225116602863104E-3</v>
       </c>
       <c r="O18">
-        <v>0.11582708155129599</v>
+        <v>0.12533379539155201</v>
       </c>
       <c r="P18">
-        <v>-0.21405282598304201</v>
+        <v>-0.14093703403793001</v>
       </c>
       <c r="Q18">
-        <v>5.8168199099966997E-2</v>
+        <v>9.5647160959361197E-2</v>
       </c>
       <c r="R18">
         <v>1</v>
       </c>
       <c r="S18">
-        <v>0.71497296180477199</v>
+        <v>0.811103054694579</v>
       </c>
       <c r="T18">
-        <v>9.5869679749665607E-3</v>
+        <v>1.0158314386439301E-2</v>
       </c>
       <c r="U18">
-        <v>-0.25978487380779203</v>
+        <v>-0.268762384402018</v>
       </c>
       <c r="V18">
-        <v>-0.24983624880993599</v>
+        <v>-0.254255713692563</v>
       </c>
       <c r="W18">
-        <v>0.15227865756619799</v>
+        <v>0.27293126835590498</v>
       </c>
       <c r="X18">
-        <v>0.132298565450819</v>
+        <v>0.160929579379048</v>
       </c>
       <c r="Y18">
-        <v>8.9724693312693005E-2</v>
+        <v>0.124801233887306</v>
       </c>
       <c r="Z18">
-        <v>8.6161408536899201E-2</v>
+        <v>0.11791541621026</v>
       </c>
       <c r="AA18">
-        <v>-0.21308243768482299</v>
-      </c>
-      <c r="AB18">
-        <v>-4.5489345349574002E-2</v>
+        <v>-0.22745841435997199</v>
       </c>
     </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>17</v>
       </c>
       <c r="B19">
-        <v>0.192340741480129</v>
+        <v>0.229596899130526</v>
       </c>
       <c r="C19">
-        <v>0.61645101991369999</v>
+        <v>0.657939912070587</v>
       </c>
       <c r="D19">
-        <v>0.68613351220254604</v>
+        <v>0.73076156845948304</v>
       </c>
       <c r="E19">
-        <v>-0.166807040029047</v>
+        <v>-0.16901237624464299</v>
       </c>
       <c r="F19">
-        <v>-0.16652478165910101</v>
+        <v>-0.16917322408693</v>
       </c>
       <c r="G19">
-        <v>-5.1605625587822397E-2</v>
+        <v>-6.2731100353620103E-2</v>
       </c>
       <c r="H19">
-        <v>-1.33711823739062E-2</v>
+        <v>-1.2467707776255501E-2</v>
       </c>
       <c r="I19">
-        <v>-1.51747032953414E-2</v>
+        <v>-3.2254653599315099E-2</v>
       </c>
       <c r="J19">
-        <v>-0.74197877818566005</v>
+        <v>-0.78979596181029998</v>
       </c>
       <c r="K19">
-        <v>-0.21253665298656299</v>
+        <v>-0.218524497327061</v>
       </c>
       <c r="L19">
-        <v>2.2611843744352799E-3</v>
+        <v>1.5704901943191E-3</v>
       </c>
       <c r="M19">
-        <v>1.6378972797373001E-3</v>
+        <v>1.1508149086765799E-4</v>
       </c>
       <c r="N19">
-        <v>1.64946348161116E-2</v>
+        <v>1.71174642466396E-2</v>
       </c>
       <c r="O19">
-        <v>0.229060892436624</v>
+        <v>0.22536653433276399</v>
       </c>
       <c r="P19">
-        <v>0.24235115251148101</v>
+        <v>0.101271099925174</v>
       </c>
       <c r="Q19">
-        <v>4.2076503206321801E-2</v>
+        <v>5.36573704086468E-2</v>
       </c>
       <c r="R19">
-        <v>0.71497296180477199</v>
+        <v>0.811103054694579</v>
       </c>
       <c r="S19">
         <v>1</v>
       </c>
       <c r="T19">
-        <v>4.94433985373213E-3</v>
+        <v>5.7324332802259704E-3</v>
       </c>
       <c r="U19">
-        <v>-0.112663795119595</v>
+        <v>-0.13630747771667501</v>
       </c>
       <c r="V19">
-        <v>-0.10437543874707</v>
+        <v>-0.13144361168170099</v>
       </c>
       <c r="W19">
-        <v>0.15049049418822499</v>
+        <v>0.19814942695975099</v>
       </c>
       <c r="X19">
-        <v>0.119791865505505</v>
+        <v>0.134255701050049</v>
       </c>
       <c r="Y19">
-        <v>-2.6920303802167801E-2</v>
+        <v>-7.5952232722702904E-3</v>
       </c>
       <c r="Z19">
-        <v>1.41609423757644E-2</v>
+        <v>2.9366514365872301E-2</v>
       </c>
       <c r="AA19">
-        <v>-0.13768951265986801</v>
-      </c>
-      <c r="AB19">
-        <v>-5.2236197096125897E-2</v>
+        <v>-0.137225134460843</v>
       </c>
     </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>18</v>
       </c>
       <c r="B20">
-        <v>9.7633047198213405E-2</v>
+        <v>9.3381194751659097E-2</v>
       </c>
       <c r="C20">
-        <v>9.2004902025702301E-3</v>
+        <v>9.2287791105834498E-3</v>
       </c>
       <c r="D20">
-        <v>1.8525892176001001E-2</v>
+        <v>1.7468997559584799E-2</v>
       </c>
       <c r="E20">
-        <v>-3.8286059098724201E-3</v>
+        <v>-3.7944865833659902E-3</v>
       </c>
       <c r="F20">
-        <v>-2.6353242269411001E-3</v>
+        <v>-2.5975808222926098E-3</v>
       </c>
       <c r="G20">
-        <v>7.06203816190909E-3</v>
+        <v>7.0548692528608703E-3</v>
       </c>
       <c r="H20">
-        <v>0.118098410497816</v>
+        <v>0.11276700276788799</v>
       </c>
       <c r="I20">
-        <v>3.1531692662043601E-2</v>
+        <v>2.7123037488918401E-2</v>
       </c>
       <c r="J20">
-        <v>-5.1377631770755904E-3</v>
+        <v>-6.6292066455728499E-3</v>
       </c>
       <c r="K20">
-        <v>-1.36880537788284E-2</v>
+        <v>-1.36056608132861E-2</v>
       </c>
       <c r="L20">
-        <v>3.2323426782878799E-3</v>
+        <v>3.2421204109885399E-3</v>
       </c>
       <c r="M20">
-        <v>1.48331205726915E-3</v>
+        <v>1.7049318855510301E-3</v>
       </c>
       <c r="N20">
-        <v>-9.5759427022190603E-4</v>
+        <v>-9.4735211482512005E-4</v>
       </c>
       <c r="O20">
-        <v>6.2911492307972296E-3</v>
+        <v>6.8507037955172403E-3</v>
       </c>
       <c r="P20">
-        <v>3.6756898156804302E-2</v>
+        <v>3.6889406369608101E-2</v>
       </c>
       <c r="Q20">
-        <v>7.0146639419401604E-3</v>
+        <v>9.8027315292476304E-3</v>
       </c>
       <c r="R20">
-        <v>9.5869679749665607E-3</v>
+        <v>1.0158314386439301E-2</v>
       </c>
       <c r="S20">
-        <v>4.94433985373213E-3</v>
+        <v>5.7324332802259704E-3</v>
       </c>
       <c r="T20">
         <v>1</v>
       </c>
       <c r="U20">
-        <v>-1.15226629131944E-2</v>
+        <v>-1.27678423823219E-2</v>
       </c>
       <c r="V20">
-        <v>-2.8582639912616298E-2</v>
+        <v>-3.0725423308818601E-2</v>
       </c>
       <c r="W20">
-        <v>5.2240122349664297E-2</v>
+        <v>4.53028878675431E-2</v>
       </c>
       <c r="X20">
-        <v>-0.15938095671983901</v>
+        <v>-0.15906216063738299</v>
       </c>
       <c r="Y20">
-        <v>3.3271143076920501E-2</v>
+        <v>3.3229137569483501E-2</v>
       </c>
       <c r="Z20">
-        <v>-0.21578206575061101</v>
+        <v>-0.21276337540965401</v>
       </c>
       <c r="AA20">
-        <v>2.7298482749117999E-2</v>
-      </c>
-      <c r="AB20">
-        <v>4.9955683897586704E-3</v>
+        <v>2.7338811125661701E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>19</v>
       </c>
       <c r="B21">
-        <v>-0.27427194530577698</v>
+        <v>-0.23121821050775701</v>
       </c>
       <c r="C21">
-        <v>-0.14680572573886</v>
+        <v>-0.149649136160553</v>
       </c>
       <c r="D21">
-        <v>-0.274135584536364</v>
+        <v>-0.244802331775438</v>
       </c>
       <c r="E21">
-        <v>6.9601065794114694E-2</v>
+        <v>8.0007392848681094E-2</v>
       </c>
       <c r="F21">
-        <v>6.6575436053175605E-2</v>
+        <v>7.6869614355027496E-2</v>
       </c>
       <c r="G21">
-        <v>-1.64518954950152E-2</v>
+        <v>-3.1698002323982101E-2</v>
       </c>
       <c r="H21">
-        <v>0.254847393876033</v>
+        <v>0.26114151985933198</v>
       </c>
       <c r="I21">
-        <v>0.53765202284186298</v>
+        <v>0.56366019776934995</v>
       </c>
       <c r="J21">
-        <v>0.40694226542013001</v>
+        <v>0.418908006946282</v>
       </c>
       <c r="K21">
-        <v>0.26245840079336002</v>
+        <v>0.281345371688493</v>
       </c>
       <c r="L21">
-        <v>2.9355293171958501E-2</v>
+        <v>2.9959979199500199E-2</v>
       </c>
       <c r="M21">
-        <v>3.1009265741002399E-2</v>
+        <v>3.2838646312183299E-2</v>
       </c>
       <c r="N21">
-        <v>-3.5319360740704103E-2</v>
+        <v>-3.5882027050311398E-2</v>
       </c>
       <c r="O21">
-        <v>7.8297070303933701E-3</v>
+        <v>1.27605333965073E-2</v>
       </c>
       <c r="P21">
-        <v>2.0003779542233001E-2</v>
+        <v>-1.1030756180542499E-3</v>
       </c>
       <c r="Q21">
-        <v>-3.8606221400018403E-2</v>
+        <v>-4.7437735153015102E-2</v>
       </c>
       <c r="R21">
-        <v>-0.25978487380779203</v>
+        <v>-0.268762384402018</v>
       </c>
       <c r="S21">
-        <v>-0.112663795119595</v>
+        <v>-0.13630747771667501</v>
       </c>
       <c r="T21">
-        <v>-1.15226629131944E-2</v>
+        <v>-1.27678423823219E-2</v>
       </c>
       <c r="U21">
         <v>1</v>
       </c>
       <c r="V21">
-        <v>0.990438615498486</v>
+        <v>0.98832062876711002</v>
       </c>
       <c r="W21">
-        <v>-0.119287398125889</v>
+        <v>-0.233807311168758</v>
       </c>
       <c r="X21">
-        <v>3.8445107593814497E-2</v>
+        <v>-1.1117485975726E-2</v>
       </c>
       <c r="Y21">
-        <v>-0.127116878892715</v>
+        <v>-0.15232905325329399</v>
       </c>
       <c r="Z21">
-        <v>-7.8322422072469006E-2</v>
+        <v>-0.11749020367622801</v>
       </c>
       <c r="AA21">
-        <v>8.7848712686390606E-2</v>
-      </c>
-      <c r="AB21">
-        <v>7.1520245489195999E-2</v>
+        <v>0.10036190108359801</v>
       </c>
     </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>20</v>
       </c>
       <c r="B22">
-        <v>-0.31246448601912002</v>
+        <v>-0.27567437110297899</v>
       </c>
       <c r="C22">
-        <v>-0.166649416939254</v>
+        <v>-0.173611531697661</v>
       </c>
       <c r="D22">
-        <v>-0.29579747228888198</v>
+        <v>-0.27149010189258199</v>
       </c>
       <c r="E22">
-        <v>3.2065359025625399E-2</v>
+        <v>3.9620112766821397E-2</v>
       </c>
       <c r="F22">
-        <v>2.88335492437807E-2</v>
+        <v>3.6206859110848803E-2</v>
       </c>
       <c r="G22">
-        <v>6.4456573214850604E-3</v>
+        <v>-5.5766781916063404E-4</v>
       </c>
       <c r="H22">
-        <v>0.26044746788297701</v>
+        <v>0.27050690871508298</v>
       </c>
       <c r="I22">
-        <v>0.54644713348316998</v>
+        <v>0.57243081326907996</v>
       </c>
       <c r="J22">
-        <v>0.41422229936285998</v>
+        <v>0.43072012751969602</v>
       </c>
       <c r="K22">
-        <v>0.24322096589928699</v>
+        <v>0.26817683671872</v>
       </c>
       <c r="L22">
-        <v>2.98324955844738E-2</v>
+        <v>3.0662008921144599E-2</v>
       </c>
       <c r="M22">
-        <v>3.3516794185490202E-2</v>
+        <v>3.6695186468913898E-2</v>
       </c>
       <c r="N22">
-        <v>-3.5503142737454203E-2</v>
+        <v>-3.66043570610717E-2</v>
       </c>
       <c r="O22">
-        <v>9.6136207107205707E-3</v>
+        <v>1.8337739530291899E-2</v>
       </c>
       <c r="P22">
-        <v>1.9454694727210099E-2</v>
+        <v>-3.4873895181731598E-3</v>
       </c>
       <c r="Q22">
-        <v>-4.2131966352810697E-2</v>
+        <v>-5.0366191334870698E-2</v>
       </c>
       <c r="R22">
-        <v>-0.24983624880993599</v>
+        <v>-0.254255713692563</v>
       </c>
       <c r="S22">
-        <v>-0.10437543874707</v>
+        <v>-0.13144361168170099</v>
       </c>
       <c r="T22">
-        <v>-2.8582639912616298E-2</v>
+        <v>-3.0725423308818601E-2</v>
       </c>
       <c r="U22">
-        <v>0.990438615498486</v>
+        <v>0.98832062876711002</v>
       </c>
       <c r="V22">
         <v>1</v>
       </c>
       <c r="W22">
-        <v>-9.2858910709228498E-2</v>
+        <v>-0.20299410568604001</v>
       </c>
       <c r="X22">
-        <v>7.6118659191074495E-2</v>
+        <v>2.9024639344177299E-2</v>
       </c>
       <c r="Y22">
-        <v>-0.107627768534484</v>
+        <v>-0.128423354907513</v>
       </c>
       <c r="Z22">
-        <v>-3.4643506744198103E-2</v>
+        <v>-6.8007372928491794E-2</v>
       </c>
       <c r="AA22">
-        <v>5.4860814525610903E-2</v>
-      </c>
-      <c r="AB22">
-        <v>6.9025749499239897E-2</v>
+        <v>6.5510932844708603E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>21</v>
       </c>
       <c r="B23">
-        <v>0.30871660314744298</v>
+        <v>0.28271681668785598</v>
       </c>
       <c r="C23">
-        <v>0.25145428235935702</v>
+        <v>0.242517664830741</v>
       </c>
       <c r="D23">
-        <v>0.29351299034254902</v>
+        <v>0.30235439958153498</v>
       </c>
       <c r="E23">
-        <v>-0.29217114663811</v>
+        <v>-0.291260818856867</v>
       </c>
       <c r="F23">
-        <v>-0.29512104598598898</v>
+        <v>-0.29421982112524397</v>
       </c>
       <c r="G23">
-        <v>0.29318972577584301</v>
+        <v>0.341083700157509</v>
       </c>
       <c r="H23">
-        <v>-0.127480137885496</v>
+        <v>-0.115392950843674</v>
       </c>
       <c r="I23">
-        <v>-0.43828925683601899</v>
+        <v>-0.498382560235619</v>
       </c>
       <c r="J23">
-        <v>-0.30903094026378802</v>
+        <v>-0.32338621823109098</v>
       </c>
       <c r="K23">
-        <v>-0.123633509631869</v>
+        <v>-0.136202597322164</v>
       </c>
       <c r="L23">
-        <v>0.119848063794434</v>
+        <v>0.10003270628434401</v>
       </c>
       <c r="M23">
-        <v>0.12367342803864199</v>
+        <v>0.10703612136876101</v>
       </c>
       <c r="N23">
-        <v>-9.8458776218714292E-4</v>
+        <v>8.0572116785610002E-4</v>
       </c>
       <c r="O23">
-        <v>0.112052903910382</v>
+        <v>0.11714739026446599</v>
       </c>
       <c r="P23">
-        <v>2.6518918379687201E-2</v>
+        <v>4.8663627356813698E-2</v>
       </c>
       <c r="Q23">
-        <v>0.120727511181492</v>
+        <v>0.13378126700394699</v>
       </c>
       <c r="R23">
-        <v>0.15227865756619799</v>
+        <v>0.27293126835590498</v>
       </c>
       <c r="S23">
-        <v>0.15049049418822499</v>
+        <v>0.19814942695975099</v>
       </c>
       <c r="T23">
-        <v>5.2240122349664297E-2</v>
+        <v>4.53028878675431E-2</v>
       </c>
       <c r="U23">
-        <v>-0.119287398125889</v>
+        <v>-0.233807311168758</v>
       </c>
       <c r="V23">
-        <v>-9.2858910709228498E-2</v>
+        <v>-0.20299410568604001</v>
       </c>
       <c r="W23">
         <v>1</v>
       </c>
       <c r="X23">
-        <v>0.46989411860642399</v>
+        <v>0.44419136315465202</v>
       </c>
       <c r="Y23">
-        <v>0.59430613916053698</v>
+        <v>0.59114463998830302</v>
       </c>
       <c r="Z23">
-        <v>0.420961502640675</v>
+        <v>0.424120805203346</v>
       </c>
       <c r="AA23">
-        <v>-0.21329793546572601</v>
-      </c>
-      <c r="AB23">
-        <v>0.131803381852202</v>
+        <v>-0.213727456748946</v>
       </c>
     </row>
-    <row r="24" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>22</v>
       </c>
       <c r="B24">
-        <v>0.106218466727422</v>
+        <v>0.11166170546317</v>
       </c>
       <c r="C24">
-        <v>0.184360914792182</v>
+        <v>0.184808441212753</v>
       </c>
       <c r="D24">
-        <v>0.155435978090565</v>
+        <v>0.15895178470000801</v>
       </c>
       <c r="E24">
-        <v>-9.7928991955129496E-2</v>
+        <v>-9.7555328419099696E-2</v>
       </c>
       <c r="F24">
-        <v>-0.10377720036309</v>
+        <v>-0.103382911920406</v>
       </c>
       <c r="G24">
-        <v>0.113515540492533</v>
+        <v>0.11358951710111399</v>
       </c>
       <c r="H24">
-        <v>-4.4181101265618999E-2</v>
+        <v>-4.5229299345927003E-2</v>
       </c>
       <c r="I24">
-        <v>-0.15803083212854099</v>
+        <v>-0.18216489085138801</v>
       </c>
       <c r="J24">
-        <v>-0.137656247078076</v>
+        <v>-0.14711573401696201</v>
       </c>
       <c r="K24">
-        <v>-0.112091492470516</v>
+        <v>-0.11019383218053699</v>
       </c>
       <c r="L24">
-        <v>0.124677379081522</v>
+        <v>0.12506885368253401</v>
       </c>
       <c r="M24">
-        <v>0.131961337303349</v>
+        <v>0.13655745890273999</v>
       </c>
       <c r="N24">
-        <v>-2.5815755942230598E-2</v>
+        <v>-2.6054096300289101E-2</v>
       </c>
       <c r="O24">
-        <v>6.81021547542391E-2</v>
+        <v>8.3290003715019906E-2</v>
       </c>
       <c r="P24">
-        <v>-1.6855431979829201E-2</v>
+        <v>-1.1529934233992701E-2</v>
       </c>
       <c r="Q24">
-        <v>0.14632188638653101</v>
+        <v>0.168862769211928</v>
       </c>
       <c r="R24">
-        <v>0.132298565450819</v>
+        <v>0.160929579379048</v>
       </c>
       <c r="S24">
-        <v>0.119791865505505</v>
+        <v>0.134255701050049</v>
       </c>
       <c r="T24">
-        <v>-0.15938095671983901</v>
+        <v>-0.15906216063738299</v>
       </c>
       <c r="U24">
-        <v>3.8445107593814497E-2</v>
+        <v>-1.1117485975726E-2</v>
       </c>
       <c r="V24">
-        <v>7.6118659191074495E-2</v>
+        <v>2.9024639344177299E-2</v>
       </c>
       <c r="W24">
-        <v>0.46989411860642399</v>
+        <v>0.44419136315465202</v>
       </c>
       <c r="X24">
         <v>1</v>
       </c>
       <c r="Y24">
-        <v>0.39307664242828</v>
+        <v>0.39639495576910799</v>
       </c>
       <c r="Z24">
-        <v>0.57865108965188405</v>
+        <v>0.58652918491761796</v>
       </c>
       <c r="AA24">
-        <v>1.2507106060828299E-2</v>
-      </c>
-      <c r="AB24">
-        <v>0.157071465957137</v>
+        <v>1.31662957014763E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>23</v>
       </c>
       <c r="B25">
-        <v>0.12832966716114799</v>
+        <v>0.11105253485494</v>
       </c>
       <c r="C25">
-        <v>0.105867381114794</v>
+        <v>0.10656092611986399</v>
       </c>
       <c r="D25">
-        <v>9.87840398923166E-2</v>
+        <v>0.10148969151331</v>
       </c>
       <c r="E25">
-        <v>-7.5401385422106906E-2</v>
+        <v>-7.4931641304289906E-2</v>
       </c>
       <c r="F25">
-        <v>-8.1589034518109296E-2</v>
+        <v>-8.1019166564176806E-2</v>
       </c>
       <c r="G25">
-        <v>0.630997245905774</v>
+        <v>0.63066920458550302</v>
       </c>
       <c r="H25">
-        <v>-0.17978042859919199</v>
+        <v>-0.175414737082462</v>
       </c>
       <c r="I25">
-        <v>-0.20103723869006701</v>
+        <v>-0.20290023437662</v>
       </c>
       <c r="J25">
-        <v>-0.143681301661506</v>
+        <v>-0.14620357332269901</v>
       </c>
       <c r="K25">
-        <v>-0.122682584322403</v>
+        <v>-0.122316539374464</v>
       </c>
       <c r="L25">
-        <v>0.17232256502187901</v>
+        <v>0.17167983096360301</v>
       </c>
       <c r="M25">
-        <v>0.17946890170118099</v>
+        <v>0.18358869007858999</v>
       </c>
       <c r="N25">
-        <v>-3.0079770288262999E-2</v>
+        <v>-3.1347358791964201E-2</v>
       </c>
       <c r="O25">
-        <v>8.1964377171543895E-2</v>
+        <v>0.10137185199915801</v>
       </c>
       <c r="P25">
-        <v>9.7546108678770605E-3</v>
+        <v>1.4238887284318E-2</v>
       </c>
       <c r="Q25">
-        <v>0.24637340129289301</v>
+        <v>0.287109185823404</v>
       </c>
       <c r="R25">
-        <v>8.9724693312693005E-2</v>
+        <v>0.124801233887306</v>
       </c>
       <c r="S25">
-        <v>-2.6920303802167801E-2</v>
+        <v>-7.5952232722702904E-3</v>
       </c>
       <c r="T25">
-        <v>3.3271143076920501E-2</v>
+        <v>3.3229137569483501E-2</v>
       </c>
       <c r="U25">
-        <v>-0.127116878892715</v>
+        <v>-0.15232905325329399</v>
       </c>
       <c r="V25">
-        <v>-0.107627768534484</v>
+        <v>-0.128423354907513</v>
       </c>
       <c r="W25">
-        <v>0.59430613916053698</v>
+        <v>0.59114463998830302</v>
       </c>
       <c r="X25">
-        <v>0.39307664242828</v>
+        <v>0.39639495576910799</v>
       </c>
       <c r="Y25">
         <v>1</v>
       </c>
       <c r="Z25">
-        <v>0.77657324840674702</v>
+        <v>0.78583124109337399</v>
       </c>
       <c r="AA25">
-        <v>-2.5494011754850499E-2</v>
-      </c>
-      <c r="AB25">
-        <v>0.220463374820492</v>
+        <v>-2.4312177522831199E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>24</v>
       </c>
       <c r="B26">
-        <v>1.36591290329088E-2</v>
+        <v>7.2011969225451696E-3</v>
       </c>
       <c r="C26">
-        <v>7.9201619499369505E-2</v>
+        <v>8.3620463458723399E-2</v>
       </c>
       <c r="D26">
-        <v>7.7058195484517797E-2</v>
+        <v>8.1089629525839604E-2</v>
       </c>
       <c r="E26">
-        <v>-9.2943492465488803E-2</v>
+        <v>-9.1718760780692202E-2</v>
       </c>
       <c r="F26">
-        <v>-9.8770921338221504E-2</v>
+        <v>-9.7546844149951906E-2</v>
       </c>
       <c r="G26">
-        <v>0.44292299487454401</v>
+        <v>0.44828804845697201</v>
       </c>
       <c r="H26">
-        <v>-0.16203001598061501</v>
+        <v>-0.162096064853503</v>
       </c>
       <c r="I26">
-        <v>-0.17282585702009701</v>
+        <v>-0.18226350128587601</v>
       </c>
       <c r="J26">
-        <v>-0.125989281254833</v>
+        <v>-0.13545280154401099</v>
       </c>
       <c r="K26">
-        <v>-0.13458667157922799</v>
+        <v>-0.13340187259202699</v>
       </c>
       <c r="L26">
-        <v>0.155322282671887</v>
+        <v>0.15923748453613401</v>
       </c>
       <c r="M26">
-        <v>0.16890930148582001</v>
+        <v>0.17732317970556299</v>
       </c>
       <c r="N26">
-        <v>-4.9360245560671298E-2</v>
+        <v>-3.98924976064313E-2</v>
       </c>
       <c r="O26">
-        <v>7.5961979969116702E-2</v>
+        <v>9.4992075329119796E-2</v>
       </c>
       <c r="P26">
-        <v>1.10871733451552E-2</v>
+        <v>7.3159325252599499E-3</v>
       </c>
       <c r="Q26">
-        <v>0.16572052342295501</v>
+        <v>0.20979604381692801</v>
       </c>
       <c r="R26">
-        <v>8.6161408536899201E-2</v>
+        <v>0.11791541621026</v>
       </c>
       <c r="S26">
-        <v>1.41609423757644E-2</v>
+        <v>2.9366514365872301E-2</v>
       </c>
       <c r="T26">
-        <v>-0.21578206575061101</v>
+        <v>-0.21276337540965401</v>
       </c>
       <c r="U26">
-        <v>-7.8322422072469006E-2</v>
+        <v>-0.11749020367622801</v>
       </c>
       <c r="V26">
-        <v>-3.4643506744198103E-2</v>
+        <v>-6.8007372928491794E-2</v>
       </c>
       <c r="W26">
-        <v>0.420961502640675</v>
+        <v>0.424120805203346</v>
       </c>
       <c r="X26">
-        <v>0.57865108965188405</v>
+        <v>0.58652918491761796</v>
       </c>
       <c r="Y26">
-        <v>0.77657324840674702</v>
+        <v>0.78583124109337399</v>
       </c>
       <c r="Z26">
         <v>1</v>
       </c>
       <c r="AA26">
-        <v>-4.3331425406412202E-2</v>
-      </c>
-      <c r="AB26">
-        <v>0.208472579452362</v>
+        <v>-3.6412651588935599E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>25</v>
       </c>
       <c r="B27">
-        <v>0.299847992281363</v>
+        <v>0.31383614451548902</v>
       </c>
       <c r="C27">
-        <v>0.33142437400341002</v>
+        <v>0.33746400655331199</v>
       </c>
       <c r="D27">
-        <v>2.88586097253971E-2</v>
+        <v>2.8091186266488499E-2</v>
       </c>
       <c r="E27">
-        <v>0.85174328645703801</v>
+        <v>0.85170465942389495</v>
       </c>
       <c r="F27">
-        <v>0.85541237804162695</v>
+        <v>0.85537912146148098</v>
       </c>
       <c r="G27">
-        <v>9.7514178750354192E-3</v>
+        <v>9.8020220511193593E-3</v>
       </c>
       <c r="H27">
-        <v>0.119790809929619</v>
+        <v>0.12558832479895801</v>
       </c>
       <c r="I27">
-        <v>4.9381628659003703E-2</v>
+        <v>5.3259383009840899E-2</v>
       </c>
       <c r="J27">
-        <v>6.5826296400070705E-2</v>
+        <v>6.8718721527367202E-2</v>
       </c>
       <c r="K27">
-        <v>-3.1815122094351403E-2</v>
+        <v>-3.1673041878570299E-2</v>
       </c>
       <c r="L27">
-        <v>8.7544496803485701E-3</v>
+        <v>8.8428071405106997E-3</v>
       </c>
       <c r="M27">
-        <v>7.4864131025065301E-3</v>
+        <v>8.3261505149158609E-3</v>
       </c>
       <c r="N27">
-        <v>-4.3183151290990297E-3</v>
+        <v>-4.32360625889974E-3</v>
       </c>
       <c r="O27">
-        <v>8.9493459482607299E-2</v>
+        <v>8.7647954435012804E-2</v>
       </c>
       <c r="P27">
-        <v>-2.2041702572722099E-2</v>
+        <v>-2.14679090719587E-2</v>
       </c>
       <c r="Q27">
-        <v>1.79028107531937E-2</v>
+        <v>2.4902457039188301E-2</v>
       </c>
       <c r="R27">
-        <v>-0.21308243768482299</v>
+        <v>-0.22745841435997199</v>
       </c>
       <c r="S27">
-        <v>-0.13768951265986801</v>
+        <v>-0.137225134460843</v>
       </c>
       <c r="T27">
-        <v>2.7298482749117999E-2</v>
+        <v>2.7338811125661701E-2</v>
       </c>
       <c r="U27">
-        <v>8.7848712686390606E-2</v>
+        <v>0.10036190108359801</v>
       </c>
       <c r="V27">
-        <v>5.4860814525610903E-2</v>
+        <v>6.5510932844708603E-2</v>
       </c>
       <c r="W27">
-        <v>-0.21329793546572601</v>
+        <v>-0.213727456748946</v>
       </c>
       <c r="X27">
-        <v>1.2507106060828299E-2</v>
+        <v>1.31662957014763E-2</v>
       </c>
       <c r="Y27">
-        <v>-2.5494011754850499E-2</v>
+        <v>-2.4312177522831199E-2</v>
       </c>
       <c r="Z27">
-        <v>-4.3331425406412202E-2</v>
+        <v>-3.6412651588935599E-2</v>
       </c>
       <c r="AA27">
-        <v>1</v>
-      </c>
-      <c r="AB27">
-        <v>0.118227750211245</v>
-      </c>
-    </row>
-    <row r="28" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>26</v>
-      </c>
-      <c r="B28">
-        <v>0.11551680549042501</v>
-      </c>
-      <c r="C28">
-        <v>8.8196514222277797E-2</v>
-      </c>
-      <c r="D28">
-        <v>4.1587117080718501E-2</v>
-      </c>
-      <c r="E28">
-        <v>0.12916707422576201</v>
-      </c>
-      <c r="F28">
-        <v>0.132520881323752</v>
-      </c>
-      <c r="G28">
-        <v>9.8158634808821102E-2</v>
-      </c>
-      <c r="H28">
-        <v>2.2949054905322602E-2</v>
-      </c>
-      <c r="I28">
-        <v>-9.2807682270836397E-2</v>
-      </c>
-      <c r="J28">
-        <v>-1.6418275480676401E-2</v>
-      </c>
-      <c r="K28">
-        <v>-7.6688667774808802E-2</v>
-      </c>
-      <c r="L28">
-        <v>-4.1470834838146502E-2</v>
-      </c>
-      <c r="M28">
-        <v>-3.7070355116631197E-2</v>
-      </c>
-      <c r="N28">
-        <v>6.8194287379843399E-2</v>
-      </c>
-      <c r="O28">
-        <v>8.5031160932701896E-2</v>
-      </c>
-      <c r="P28">
-        <v>3.2852948162221701E-2</v>
-      </c>
-      <c r="Q28">
-        <v>0.18393054966036501</v>
-      </c>
-      <c r="R28">
-        <v>-4.5489345349574002E-2</v>
-      </c>
-      <c r="S28">
-        <v>-5.2236197096125897E-2</v>
-      </c>
-      <c r="T28">
-        <v>4.9955683897586704E-3</v>
-      </c>
-      <c r="U28">
-        <v>7.1520245489195999E-2</v>
-      </c>
-      <c r="V28">
-        <v>6.9025749499239897E-2</v>
-      </c>
-      <c r="W28">
-        <v>0.131803381852202</v>
-      </c>
-      <c r="X28">
-        <v>0.157071465957137</v>
-      </c>
-      <c r="Y28">
-        <v>0.220463374820492</v>
-      </c>
-      <c r="Z28">
-        <v>0.208472579452362</v>
-      </c>
-      <c r="AA28">
-        <v>0.118227750211245</v>
-      </c>
-      <c r="AB28">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:AB28">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="greaterThan">
-      <formula>0.7</formula>
+  <conditionalFormatting sqref="B2:AA27">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>